<commit_message>
Now also counting the number of NMACs correctly.
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -451,7 +451,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,6 +503,21 @@
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="C3" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -511,6 +526,21 @@
       <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -579,7 +609,7 @@
         <v>34</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,7 +655,7 @@
         <v>34</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,7 +678,7 @@
         <v>39</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +706,7 @@
       </c>
       <c r="I13" s="3" t="n">
         <f aca="false">AVERAGE(I8:I12)</f>
-        <v>10.8</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,7 +731,7 @@
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(I8:I12)</f>
-        <v>2.56124969497314</v>
+        <v>2.57681974534503</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,6 +770,21 @@
       <c r="B17" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="C17" s="0" t="n">
+        <v>274</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -862,7 +907,7 @@
         <v>37</v>
       </c>
       <c r="I25" s="0" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,7 +930,7 @@
         <v>40</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,7 +958,7 @@
       </c>
       <c r="I27" s="3" t="n">
         <f aca="false">AVERAGE(I22:I26)</f>
-        <v>22.6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +983,7 @@
       </c>
       <c r="I28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(I22:I26)</f>
-        <v>2.57681974534502</v>
+        <v>2.44948974278318</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Now also calculating average distance flown and average flying time.
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -451,7 +451,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -506,6 +506,12 @@
       <c r="C3" s="0" t="n">
         <v>196</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>3792.94</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>311.7</v>
+      </c>
       <c r="F3" s="0" t="n">
         <v>76</v>
       </c>
@@ -529,6 +535,12 @@
       <c r="C4" s="0" t="n">
         <v>201</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>3544.49</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>300.45</v>
+      </c>
       <c r="F4" s="0" t="n">
         <v>68</v>
       </c>
@@ -576,6 +588,12 @@
       <c r="C8" s="0" t="n">
         <v>205</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>3674.95</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>324.43</v>
+      </c>
       <c r="F8" s="0" t="n">
         <v>62</v>
       </c>
@@ -599,6 +617,12 @@
       <c r="C9" s="0" t="n">
         <v>198</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>3622.18</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>300.22</v>
+      </c>
       <c r="F9" s="0" t="n">
         <v>65</v>
       </c>
@@ -622,6 +646,12 @@
       <c r="C10" s="0" t="n">
         <v>196</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>3624.6</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>301.559</v>
+      </c>
       <c r="F10" s="0" t="n">
         <v>69</v>
       </c>
@@ -644,6 +674,12 @@
       </c>
       <c r="C11" s="0" t="n">
         <v>204</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>3650.35</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>310.95</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>64</v>
@@ -667,6 +703,12 @@
       </c>
       <c r="C12" s="0" t="n">
         <v>201</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>3524.76</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>300.74</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>66</v>
@@ -690,8 +732,14 @@
         <f aca="false">AVERAGE(C8:C12)</f>
         <v>200.8</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="3" t="n">
+        <f aca="false">AVERAGE(D8:D12)</f>
+        <v>3619.368</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <f aca="false">AVERAGE(E8:E12)</f>
+        <v>307.5798</v>
+      </c>
       <c r="F13" s="3" t="n">
         <f aca="false">AVERAGE(F8:F12)</f>
         <v>65.2</v>
@@ -773,6 +821,12 @@
       <c r="C17" s="0" t="n">
         <v>274</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <v>1868.03</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>233.11</v>
+      </c>
       <c r="F17" s="0" t="n">
         <v>85</v>
       </c>
@@ -828,6 +882,12 @@
       <c r="C22" s="0" t="n">
         <v>239</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <v>1783.16</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>233.719</v>
+      </c>
       <c r="F22" s="0" t="n">
         <v>84</v>
       </c>
@@ -851,6 +911,12 @@
       <c r="C23" s="0" t="n">
         <v>267</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <v>1725.47</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>238.136</v>
+      </c>
       <c r="F23" s="0" t="n">
         <v>60</v>
       </c>
@@ -874,6 +940,12 @@
       <c r="C24" s="0" t="n">
         <v>276</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <v>1720.94</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>235.07</v>
+      </c>
       <c r="F24" s="0" t="n">
         <v>104</v>
       </c>
@@ -896,6 +968,12 @@
       </c>
       <c r="C25" s="0" t="n">
         <v>277</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>1658.64</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>230.76</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>60</v>
@@ -919,6 +997,12 @@
       </c>
       <c r="C26" s="0" t="n">
         <v>267</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1659</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>222.508</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>76</v>
@@ -942,8 +1026,14 @@
         <f aca="false">AVERAGE(C22:C26)</f>
         <v>265.2</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="3" t="n">
+        <f aca="false">AVERAGE(D22:D26)</f>
+        <v>1709.442</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <f aca="false">AVERAGE(E22:E26)</f>
+        <v>232.0386</v>
+      </c>
       <c r="F27" s="3" t="n">
         <f aca="false">AVERAGE(F22:F26)</f>
         <v>76.8</v>

</xml_diff>

<commit_message>
Filtered out duplicate CPA events.
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -451,7 +451,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -720,7 +720,7 @@
         <v>39</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,7 +754,7 @@
       </c>
       <c r="I13" s="3" t="n">
         <f aca="false">AVERAGE(I8:I12)</f>
-        <v>10.6</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,7 +779,7 @@
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(I8:I12)</f>
-        <v>2.57681974534503</v>
+        <v>2.65329983228432</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -837,7 +837,7 @@
         <v>47</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,7 +898,7 @@
         <v>54</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,7 +956,7 @@
         <v>62</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="I27" s="3" t="n">
         <f aca="false">AVERAGE(I22:I26)</f>
-        <v>23</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="I28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(I22:I26)</f>
-        <v>2.44948974278318</v>
+        <v>1.85472369909914</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Now calculating average conflict duration as well.
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="18">
   <si>
     <t xml:space="preserve">Exercise 3 statistics</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t xml:space="preserve">Conflicts resolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average conflict time</t>
   </si>
   <si>
     <t xml:space="preserve">Average</t>
@@ -195,7 +198,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="H25 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -448,10 +451,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,6 +463,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="19.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,9 +494,12 @@
         <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -519,9 +526,12 @@
         <v>76</v>
       </c>
       <c r="H3" s="0" t="n">
+        <v>6.039</v>
+      </c>
+      <c r="I3" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>6</v>
       </c>
     </row>
@@ -548,9 +558,12 @@
         <v>68</v>
       </c>
       <c r="H4" s="0" t="n">
+        <v>12.88</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -601,9 +614,12 @@
         <v>61</v>
       </c>
       <c r="H8" s="0" t="n">
+        <v>7.06</v>
+      </c>
+      <c r="I8" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>9</v>
       </c>
     </row>
@@ -630,9 +646,12 @@
         <v>65</v>
       </c>
       <c r="H9" s="0" t="n">
+        <v>7.846</v>
+      </c>
+      <c r="I9" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="J9" s="0" t="n">
         <v>13</v>
       </c>
     </row>
@@ -659,9 +678,12 @@
         <v>69</v>
       </c>
       <c r="H10" s="0" t="n">
+        <v>7.318</v>
+      </c>
+      <c r="I10" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="J10" s="0" t="n">
         <v>7</v>
       </c>
     </row>
@@ -688,9 +710,12 @@
         <v>63</v>
       </c>
       <c r="H11" s="0" t="n">
+        <v>8.079</v>
+      </c>
+      <c r="I11" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="J11" s="0" t="n">
         <v>14</v>
       </c>
     </row>
@@ -716,16 +741,19 @@
       <c r="G12" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="2" t="n">
+        <v>11.33333</v>
+      </c>
+      <c r="I12" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="J12" s="0" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="n">
@@ -750,16 +778,20 @@
       </c>
       <c r="H13" s="3" t="n">
         <f aca="false">AVERAGE(H8:H12)</f>
-        <v>35.2</v>
+        <v>8.327266</v>
       </c>
       <c r="I13" s="3" t="n">
         <f aca="false">AVERAGE(I8:I12)</f>
+        <v>35.2</v>
+      </c>
+      <c r="J13" s="3" t="n">
+        <f aca="false">AVERAGE(J8:J12)</f>
         <v>10.4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(C8:C12)</f>
@@ -773,12 +805,12 @@
         <f aca="false">_xlfn.STDEV.P(G8:G12)</f>
         <v>2.71293199325011</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">_xlfn.STDEV.P(H8:H12)</f>
-        <v>2.13541565040626</v>
-      </c>
       <c r="I14" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(I8:I12)</f>
+        <v>2.13541565040626</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(J8:J12)</f>
         <v>2.65329983228432</v>
       </c>
     </row>
@@ -804,10 +836,10 @@
       <c r="G16" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="I16" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="J16" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -834,9 +866,12 @@
         <v>84</v>
       </c>
       <c r="H17" s="0" t="n">
+        <v>16.595</v>
+      </c>
+      <c r="I17" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="J17" s="0" t="n">
         <v>15</v>
       </c>
     </row>
@@ -895,9 +930,12 @@
         <v>82</v>
       </c>
       <c r="H22" s="0" t="n">
+        <v>13.207</v>
+      </c>
+      <c r="I22" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="J22" s="0" t="n">
         <v>19</v>
       </c>
     </row>
@@ -924,9 +962,12 @@
         <v>59</v>
       </c>
       <c r="H23" s="0" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="I23" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="J23" s="0" t="n">
         <v>20</v>
       </c>
     </row>
@@ -953,9 +994,12 @@
         <v>100</v>
       </c>
       <c r="H24" s="0" t="n">
+        <v>8.73</v>
+      </c>
+      <c r="I24" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="J24" s="0" t="n">
         <v>23</v>
       </c>
     </row>
@@ -981,10 +1025,10 @@
       <c r="G25" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="I25" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="J25" s="0" t="n">
         <v>21</v>
       </c>
     </row>
@@ -1011,15 +1055,18 @@
         <v>75</v>
       </c>
       <c r="H26" s="0" t="n">
+        <v>6.23</v>
+      </c>
+      <c r="I26" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="J26" s="0" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="n">
@@ -1044,16 +1091,20 @@
       </c>
       <c r="H27" s="3" t="n">
         <f aca="false">AVERAGE(H22:H26)</f>
-        <v>45</v>
+        <v>9.31675</v>
       </c>
       <c r="I27" s="3" t="n">
         <f aca="false">AVERAGE(I22:I26)</f>
+        <v>45</v>
+      </c>
+      <c r="J27" s="3" t="n">
+        <f aca="false">AVERAGE(J22:J26)</f>
         <v>21.4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(C22:C26)</f>
@@ -1067,18 +1118,18 @@
         <f aca="false">_xlfn.STDEV.P(G22:G26)</f>
         <v>15.612815249019</v>
       </c>
-      <c r="H28" s="0" t="n">
-        <f aca="false">_xlfn.STDEV.P(H22:H26)</f>
-        <v>11.2071405808975</v>
-      </c>
       <c r="I28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(I22:I26)</f>
+        <v>11.2071405808975</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(J22:J26)</f>
         <v>1.85472369909914</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1100,7 +1151,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="H25 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added calculations of average speed.
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Low traffic densit" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="18">
   <si>
     <t xml:space="preserve">Exercise 3 statistics</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t xml:space="preserve">Average flying time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average speed</t>
   </si>
   <si>
     <t xml:space="preserve">Conflicts</t>
@@ -163,9 +166,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -213,20 +220,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -250,7 +257,7 @@
       <c r="E2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="0" t="s">
@@ -262,33 +269,40 @@
       <c r="I2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>4658.53</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>370.5</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
+        <f aca="false">D3/E3</f>
+        <v>12.5736302294197</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="H3" s="2" t="n">
         <v>10.8</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="J3" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -297,27 +311,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="2" t="n">
         <v>4350.87</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>331.61</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
+        <f aca="false">D4/E4</f>
+        <v>13.1204426887006</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="H4" s="2" t="n">
         <v>6.5</v>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -326,27 +344,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="2" t="n">
         <v>4563.4</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>343.92</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
+        <f aca="false">D5/E5</f>
+        <v>13.2687834380088</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="H5" s="2" t="n">
         <v>10.67</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="I5" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="J5" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -355,27 +377,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="2" t="n">
         <v>4541</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>348.35</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
+        <f aca="false">D6/E6</f>
+        <v>13.0357399167504</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="H6" s="2" t="n">
         <v>11.8</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="I6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="J6" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -384,27 +410,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="2" t="n">
         <v>4617.47</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>390.36</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="2" t="n">
+        <f aca="false">D7/E7</f>
+        <v>11.8287478225228</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="H7" s="2" t="n">
         <v>13.33</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="I7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="J7" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -413,27 +443,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="2" t="n">
         <v>5064.1</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>395.9</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="n">
+        <f aca="false">D8/E8</f>
+        <v>12.7913614549129</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="H8" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="H8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2" t="n">
+      <c r="I8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -442,7 +476,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>23</v>
@@ -450,19 +484,23 @@
       <c r="D9" s="0" t="n">
         <v>4524.05</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>361.99</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
+        <f aca="false">D9/E9</f>
+        <v>12.4977209315174</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="H9" s="2" t="n">
         <v>6.5</v>
       </c>
-      <c r="H9" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2" t="n">
+      <c r="I9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -471,27 +509,31 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="2" t="n">
         <v>4342.3</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>380.15</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
+        <f aca="false">D10/E10</f>
+        <v>11.4225963435486</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="H10" s="2" t="n">
         <v>6.33</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="I10" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="I10" s="2" t="n">
+      <c r="J10" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -500,27 +542,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="2" t="n">
         <v>4989.65</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="2" t="n">
         <v>376.24</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="2" t="n">
+        <f aca="false">D11/E11</f>
+        <v>13.2618807144376</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="H11" s="2" t="n">
         <v>6.5</v>
       </c>
-      <c r="H11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="n">
+      <c r="I11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -529,7 +575,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>28</v>
@@ -537,59 +583,67 @@
       <c r="D12" s="0" t="n">
         <v>4742.65</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="2" t="n">
         <v>388.91</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="2" t="n">
+        <f aca="false">D12/E12</f>
+        <v>12.1947237149983</v>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="H12" s="5" t="n">
         <v>6.5</v>
       </c>
-      <c r="H12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2" t="n">
+      <c r="I12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="n">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7" t="n">
         <f aca="false">AVERAGE(C3:C12)</f>
         <v>25.2</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="7" t="n">
         <f aca="false">AVERAGE(D3:D12)</f>
         <v>4639.402</v>
       </c>
-      <c r="E13" s="6" t="n">
+      <c r="E13" s="7" t="n">
         <f aca="false">AVERAGE(E3:E12)</f>
         <v>368.793</v>
       </c>
-      <c r="F13" s="6" t="n">
-        <f aca="false">AVERAGE(F3:F12)</f>
+      <c r="F13" s="7" t="n">
+        <f aca="false">AVERAGE(F3:F11)</f>
+        <v>12.6445448377576</v>
+      </c>
+      <c r="G13" s="7" t="n">
+        <f aca="false">AVERAGE(G3:G12)</f>
         <v>3.3</v>
       </c>
-      <c r="G13" s="6" t="n">
-        <f aca="false">AVERAGE(G3:G12)</f>
+      <c r="H13" s="7" t="n">
+        <f aca="false">AVERAGE(H3:H12)</f>
         <v>8.493</v>
       </c>
-      <c r="H13" s="6" t="n">
-        <f aca="false">AVERAGE(H3:H12)</f>
+      <c r="I13" s="7" t="n">
+        <f aca="false">AVERAGE(I3:I12)</f>
         <v>2.2</v>
       </c>
-      <c r="I13" s="6" t="n">
-        <f aca="false">AVERAGE(I3:I12)</f>
+      <c r="J13" s="7" t="n">
+        <f aca="false">AVERAGE(J3:J12)</f>
         <v>0.7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(C3:C12)</f>
@@ -603,20 +657,24 @@
         <f aca="false">_xlfn.STDEV.P(E3:E12)</f>
         <v>20.6334931846258</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F3:F12)</f>
-        <v>1.41774468787578</v>
+        <v>0.594913360081156</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(G3:G12)</f>
-        <v>2.66788699160965</v>
+        <v>1.41774468787578</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(H3:H12)</f>
-        <v>1.46969384566991</v>
+        <v>2.66788699160965</v>
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(I3:I12)</f>
+        <v>1.46969384566991</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(J3:J12)</f>
         <v>0.458257569495584</v>
       </c>
     </row>
@@ -636,7 +694,7 @@
       <c r="E16" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="0" t="s">
@@ -648,33 +706,40 @@
       <c r="I16" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="J16" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="2" t="n">
         <v>2592.22</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="2" t="n">
         <v>267.42</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="2" t="n">
+        <f aca="false">D17/E17</f>
+        <v>9.69344102909281</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G17" s="1" t="n">
+      <c r="H17" s="2" t="n">
         <v>12.75</v>
       </c>
-      <c r="H17" s="2" t="n">
+      <c r="I17" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I17" s="2" t="n">
+      <c r="J17" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -682,28 +747,32 @@
       <c r="A18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>13</v>
+      <c r="B18" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="2" t="n">
         <v>2234.42</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="2" t="n">
         <v>252.39</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="2" t="n">
+        <f aca="false">D18/E18</f>
+        <v>8.85304489084354</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="H18" s="2" t="n">
         <v>11.5</v>
       </c>
-      <c r="H18" s="2" t="n">
+      <c r="I18" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="I18" s="2" t="n">
+      <c r="J18" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -711,28 +780,32 @@
       <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>13</v>
+      <c r="B19" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="2" t="n">
         <v>3028.08</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="2" t="n">
         <v>275.35</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="2" t="n">
+        <f aca="false">D19/E19</f>
+        <v>10.9972035591066</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G19" s="1" t="n">
+      <c r="H19" s="2" t="n">
         <v>7.83</v>
       </c>
-      <c r="H19" s="2" t="n">
+      <c r="I19" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="I19" s="2" t="n">
+      <c r="J19" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -740,28 +813,32 @@
       <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>13</v>
+      <c r="B20" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="2" t="n">
         <v>2514.8</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="2" t="n">
         <v>267.29</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="2" t="n">
+        <f aca="false">D20/E20</f>
+        <v>9.40850761345355</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="H20" s="2" t="n">
         <v>11.17</v>
       </c>
-      <c r="H20" s="2" t="n">
+      <c r="I20" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="I20" s="2" t="n">
+      <c r="J20" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -769,28 +846,32 @@
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>13</v>
+      <c r="B21" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="2" t="n">
         <v>2289.49</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="2" t="n">
         <v>249.01</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="2" t="n">
+        <f aca="false">D21/E21</f>
+        <v>9.19436970402795</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="H21" s="2" t="n">
         <v>11.57</v>
       </c>
-      <c r="H21" s="2" t="n">
+      <c r="I21" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="I21" s="2" t="n">
+      <c r="J21" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -798,28 +879,32 @@
       <c r="A22" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>13</v>
+      <c r="B22" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="2" t="n">
         <v>2836.64</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="2" t="n">
         <v>285.38</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="2" t="n">
+        <f aca="false">D22/E22</f>
+        <v>9.93986964748756</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G22" s="1" t="n">
+      <c r="H22" s="2" t="n">
         <v>6.75</v>
       </c>
-      <c r="H22" s="2" t="n">
+      <c r="I22" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="I22" s="2" t="n">
+      <c r="J22" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -827,28 +912,32 @@
       <c r="A23" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>13</v>
+      <c r="B23" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="2" t="n">
         <v>2751.56</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="2" t="n">
         <v>279.01</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="2" t="n">
+        <f aca="false">D23/E23</f>
+        <v>9.86186875022401</v>
+      </c>
+      <c r="G23" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G23" s="1" t="n">
+      <c r="H23" s="2" t="n">
         <v>6.5</v>
       </c>
-      <c r="H23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2" t="n">
+      <c r="I23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -856,28 +945,32 @@
       <c r="A24" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>13</v>
+      <c r="B24" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="2" t="n">
         <v>2624.75</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" s="2" t="n">
         <v>279.87</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="2" t="n">
+        <f aca="false">D24/E24</f>
+        <v>9.37846142852039</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G24" s="1" t="n">
+      <c r="H24" s="2" t="n">
         <v>6.5</v>
       </c>
-      <c r="H24" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" s="2" t="n">
+      <c r="I24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -885,28 +978,32 @@
       <c r="A25" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>13</v>
+      <c r="B25" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="2" t="n">
         <v>2911.88</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="2" t="n">
         <v>301.15</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="2" t="n">
+        <f aca="false">D25/E25</f>
+        <v>9.66920139465383</v>
+      </c>
+      <c r="G25" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G25" s="1" t="n">
+      <c r="H25" s="2" t="n">
         <v>5.75</v>
       </c>
-      <c r="H25" s="2" t="n">
+      <c r="I25" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="I25" s="2" t="n">
+      <c r="J25" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -914,68 +1011,76 @@
       <c r="A26" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>13</v>
+      <c r="B26" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="2" t="n">
         <v>2348.9</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" s="2" t="n">
         <v>258.78</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="2" t="n">
+        <f aca="false">D26/E26</f>
+        <v>9.07682201097457</v>
+      </c>
+      <c r="G26" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="H26" s="2" t="n">
         <v>7.6</v>
       </c>
-      <c r="H26" s="2" t="n">
+      <c r="I26" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="I26" s="2" t="n">
+      <c r="J26" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6" t="n">
+      <c r="A27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7" t="n">
         <f aca="false">AVERAGE(C17:C26)</f>
         <v>38.9</v>
       </c>
-      <c r="D27" s="6" t="n">
+      <c r="D27" s="7" t="n">
         <f aca="false">AVERAGE(D17:D26)</f>
         <v>2613.274</v>
       </c>
-      <c r="E27" s="6" t="n">
+      <c r="E27" s="7" t="n">
         <f aca="false">AVERAGE(E17:E26)</f>
         <v>271.565</v>
       </c>
-      <c r="F27" s="6" t="n">
+      <c r="F27" s="7" t="n">
         <f aca="false">AVERAGE(F17:F26)</f>
+        <v>9.60727900283848</v>
+      </c>
+      <c r="G27" s="7" t="n">
+        <f aca="false">AVERAGE(G17:G26)</f>
         <v>4.6</v>
       </c>
-      <c r="G27" s="6" t="n">
-        <f aca="false">AVERAGE(G17:G26)</f>
+      <c r="H27" s="7" t="n">
+        <f aca="false">AVERAGE(H17:H26)</f>
         <v>8.792</v>
       </c>
-      <c r="H27" s="6" t="n">
-        <f aca="false">AVERAGE(H17:H26)</f>
+      <c r="I27" s="7" t="n">
+        <f aca="false">AVERAGE(I17:I26)</f>
         <v>3.6</v>
       </c>
-      <c r="I27" s="6" t="n">
-        <f aca="false">AVERAGE(I17:I26)</f>
+      <c r="J27" s="7" t="n">
+        <f aca="false">AVERAGE(J17:J26)</f>
         <v>1.1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(C17:C26)</f>
@@ -989,20 +1094,24 @@
         <f aca="false">_xlfn.STDEV.P(E17:E26)</f>
         <v>15.1002491701296</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F17:F26)</f>
-        <v>1.62480768092719</v>
+        <v>0.568436133473986</v>
       </c>
       <c r="G28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(G17:G26)</f>
-        <v>2.50294946013698</v>
+        <v>1.62480768092719</v>
       </c>
       <c r="H28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(H17:H26)</f>
-        <v>1.68522995463527</v>
+        <v>2.50294946013698</v>
       </c>
       <c r="I28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(I17:I26)</f>
+        <v>1.68522995463527</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <f aca="false">_xlfn.STDEV.P(J17:J26)</f>
         <v>0.7</v>
       </c>
     </row>
@@ -1022,20 +1131,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,26 +1159,29 @@
       <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,27 +1189,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>195</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>3812.39</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>313.3</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
+        <f aca="false">D3/E3</f>
+        <v>12.1684966485796</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="H3" s="2" t="n">
         <v>6.85</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1106,27 +1222,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="2" t="n">
         <v>3562.22</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>301.96</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
+        <f aca="false">D4/E4</f>
+        <v>11.7969929792025</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="H4" s="2" t="n">
         <v>14.13</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1135,27 +1255,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>199</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="2" t="n">
         <v>3617.58</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>289.68</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
+        <f aca="false">D5/E5</f>
+        <v>12.4881938690969</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="H5" s="2" t="n">
         <v>25.36</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1164,27 +1288,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>196</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="2" t="n">
         <v>3639.11</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>297.92</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
+        <f aca="false">D6/E6</f>
+        <v>12.2150577336198</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="H6" s="2" t="n">
         <v>9.58</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1193,27 +1321,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>194</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="2" t="n">
         <v>3649.09</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>291.61</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="2" t="n">
+        <f aca="false">D7/E7</f>
+        <v>12.513596927403</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="H7" s="2" t="n">
         <v>14.83</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>12</v>
       </c>
     </row>
@@ -1222,27 +1354,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>204</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="2" t="n">
         <v>3692.97</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>326.02</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="n">
+        <f aca="false">D8/E8</f>
+        <v>11.3274338997608</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="H8" s="2" t="n">
         <v>7.84</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1251,27 +1387,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>196</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="2" t="n">
         <v>3659.14</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>303.29</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
+        <f aca="false">D9/E9</f>
+        <v>12.0648224471628</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="H9" s="2" t="n">
         <v>8.95</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="I9" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="J9" s="0" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1280,27 +1420,31 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>194</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="2" t="n">
         <v>3661.97</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>304.67</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
+        <f aca="false">D10/E10</f>
+        <v>12.0194636820166</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="H10" s="2" t="n">
         <v>9.71</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="J10" s="0" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1309,27 +1453,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>202</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="2" t="n">
         <v>3686.5</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="2" t="n">
         <v>314.03</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="2" t="n">
+        <f aca="false">D11/E11</f>
+        <v>11.739324268382</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="H11" s="2" t="n">
         <v>9.78</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="I11" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="J11" s="0" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1338,94 +1486,106 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>199</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="2" t="n">
         <v>3560.19</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="2" t="n">
         <v>303.76</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="2" t="n">
+        <f aca="false">D12/E12</f>
+        <v>11.7204042665262</v>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="H12" s="5" t="n">
         <v>12.26</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="I12" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="J12" s="0" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="n">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7" t="n">
         <f aca="false">AVERAGE(C3:C12)</f>
         <v>197.9</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="7" t="n">
         <f aca="false">AVERAGE(D3:D12)</f>
         <v>3654.116</v>
       </c>
-      <c r="E13" s="6" t="n">
+      <c r="E13" s="7" t="n">
         <f aca="false">AVERAGE(E3:E12)</f>
         <v>304.624</v>
       </c>
-      <c r="F13" s="6" t="n">
-        <f aca="false">AVERAGE(F3:F12)</f>
+      <c r="F13" s="7" t="n">
+        <f aca="false">AVERAGE(F3:F11)</f>
+        <v>12.0370424950249</v>
+      </c>
+      <c r="G13" s="7" t="n">
+        <f aca="false">AVERAGE(G3:G12)</f>
         <v>56.8</v>
       </c>
-      <c r="G13" s="6" t="n">
-        <f aca="false">AVERAGE(G3:G12)</f>
+      <c r="H13" s="7" t="n">
+        <f aca="false">AVERAGE(H3:H12)</f>
         <v>11.929</v>
       </c>
-      <c r="H13" s="6" t="n">
-        <f aca="false">AVERAGE(H3:H12)</f>
+      <c r="I13" s="7" t="n">
+        <f aca="false">AVERAGE(I3:I12)</f>
         <v>35.1</v>
       </c>
-      <c r="I13" s="6" t="n">
-        <f aca="false">AVERAGE(I3:I12)</f>
+      <c r="J13" s="7" t="n">
+        <f aca="false">AVERAGE(J3:J12)</f>
         <v>9.3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(C3:C12)</f>
         <v>3.26955654485436</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(D3:D12)</f>
         <v>68.2262633008726</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(E3:E12)</f>
         <v>10.3382331178978</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F3:F12)</f>
+        <v>0.349389483439253</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.P(G3:G12)</f>
         <v>5.4</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">_xlfn.STDEV.P(G3:G12)</f>
+      <c r="H14" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.P(H3:H12)</f>
         <v>5.10109880319917</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">_xlfn.STDEV.P(H3:H12)</f>
+      <c r="I14" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.P(I3:I12)</f>
         <v>3.04795013082563</v>
       </c>
-      <c r="I14" s="0" t="n">
-        <f aca="false">_xlfn.STDEV.P(I3:I12)</f>
+      <c r="J14" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.P(J3:J12)</f>
         <v>2.96816441593117</v>
       </c>
     </row>
@@ -1436,26 +1596,29 @@
       <c r="B16" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,27 +1626,31 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>266</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="2" t="n">
         <v>1924.21</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="2" t="n">
         <v>240.13</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="2" t="n">
+        <f aca="false">D17/E17</f>
+        <v>8.01320118269271</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>77</v>
       </c>
-      <c r="G17" s="1" t="n">
+      <c r="H17" s="2" t="n">
         <v>18.1</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="I17" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="J17" s="0" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1491,28 +1658,32 @@
       <c r="A18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>13</v>
+      <c r="B18" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>224</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="2" t="n">
         <v>1746.93</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="2" t="n">
         <v>233.07</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="2" t="n">
+        <f aca="false">D18/E18</f>
+        <v>7.49530184064873</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="H18" s="2" t="n">
         <v>18.1</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="I18" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="J18" s="0" t="n">
         <v>17</v>
       </c>
     </row>
@@ -1520,28 +1691,32 @@
       <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>13</v>
+      <c r="B19" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>243</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="2" t="n">
         <v>1795.29</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="2" t="n">
         <v>231.27</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="2" t="n">
+        <f aca="false">D19/E19</f>
+        <v>7.76274484368919</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="G19" s="1" t="n">
+      <c r="H19" s="2" t="n">
         <v>18.23</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="I19" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="J19" s="0" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1549,28 +1724,32 @@
       <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>13</v>
+      <c r="B20" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>237</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="2" t="n">
         <v>1820.76</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="2" t="n">
         <v>238.72</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="2" t="n">
+        <f aca="false">D20/E20</f>
+        <v>7.62717828418231</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="H20" s="2" t="n">
         <v>16.29</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="I20" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="J20" s="0" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1578,28 +1757,32 @@
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>13</v>
+      <c r="B21" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>262</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="2" t="n">
         <v>1694.28</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="2" t="n">
         <v>219.79</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="2" t="n">
+        <f aca="false">D21/E21</f>
+        <v>7.70863096592202</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="H21" s="2" t="n">
         <v>12.27</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="I21" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="J21" s="0" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1607,28 +1790,32 @@
       <c r="A22" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>13</v>
+      <c r="B22" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>232</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="D22" s="2" t="n">
         <v>1836.97</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="2" t="n">
         <v>240.77</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="2" t="n">
+        <f aca="false">D22/E22</f>
+        <v>7.62956348382274</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="G22" s="1" t="n">
+      <c r="H22" s="2" t="n">
         <v>16.16</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="I22" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="J22" s="0" t="n">
         <v>22</v>
       </c>
     </row>
@@ -1636,28 +1823,32 @@
       <c r="A23" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>13</v>
+      <c r="B23" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>263</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="2" t="n">
         <v>1751.72</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="2" t="n">
         <v>241.76</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="2" t="n">
+        <f aca="false">D23/E23</f>
+        <v>7.24569821310391</v>
+      </c>
+      <c r="G23" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="G23" s="1" t="n">
+      <c r="H23" s="2" t="n">
         <v>11.19</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="I23" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="J23" s="0" t="n">
         <v>19</v>
       </c>
     </row>
@@ -1665,28 +1856,32 @@
       <c r="A24" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>13</v>
+      <c r="B24" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>279</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="2" t="n">
         <v>1759.18</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" s="2" t="n">
         <v>240.3</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="2" t="n">
+        <f aca="false">D24/E24</f>
+        <v>7.32076570952976</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="G24" s="1" t="n">
+      <c r="H24" s="2" t="n">
         <v>10.78</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="I24" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="J24" s="0" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1694,28 +1889,32 @@
       <c r="A25" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>13</v>
+      <c r="B25" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>272</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="2" t="n">
         <v>1689.13</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="2" t="n">
         <v>235.01</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="2" t="n">
+        <f aca="false">D25/E25</f>
+        <v>7.1874813837709</v>
+      </c>
+      <c r="G25" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="G25" s="1" t="n">
+      <c r="H25" s="2" t="n">
         <v>7.13</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="I25" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="J25" s="0" t="n">
         <v>21</v>
       </c>
     </row>
@@ -1723,101 +1922,113 @@
       <c r="A26" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>13</v>
+      <c r="B26" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>262</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="2" t="n">
         <v>1690.66</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" s="2" t="n">
         <v>226.75</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="2" t="n">
+        <f aca="false">D26/E26</f>
+        <v>7.45605292171996</v>
+      </c>
+      <c r="G26" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="H26" s="2" t="n">
         <v>7.3</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="I26" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="J26" s="0" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6" t="n">
+      <c r="A27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7" t="n">
         <f aca="false">AVERAGE(C17:C26)</f>
         <v>254</v>
       </c>
-      <c r="D27" s="6" t="n">
+      <c r="D27" s="7" t="n">
         <f aca="false">AVERAGE(D17:D26)</f>
         <v>1770.913</v>
       </c>
-      <c r="E27" s="6" t="n">
+      <c r="E27" s="7" t="n">
         <f aca="false">AVERAGE(E17:E26)</f>
         <v>234.757</v>
       </c>
-      <c r="F27" s="6" t="n">
+      <c r="F27" s="7" t="n">
         <f aca="false">AVERAGE(F17:F26)</f>
+        <v>7.54466188290822</v>
+      </c>
+      <c r="G27" s="7" t="n">
+        <f aca="false">AVERAGE(G17:G26)</f>
         <v>65.7</v>
       </c>
-      <c r="G27" s="6" t="n">
-        <f aca="false">AVERAGE(G17:G26)</f>
+      <c r="H27" s="7" t="n">
+        <f aca="false">AVERAGE(H17:H26)</f>
         <v>13.555</v>
       </c>
-      <c r="H27" s="6" t="n">
-        <f aca="false">AVERAGE(H17:H26)</f>
+      <c r="I27" s="7" t="n">
+        <f aca="false">AVERAGE(I17:I26)</f>
         <v>46.7</v>
       </c>
-      <c r="I27" s="6" t="n">
-        <f aca="false">AVERAGE(I17:I26)</f>
+      <c r="J27" s="7" t="n">
+        <f aca="false">AVERAGE(J17:J26)</f>
         <v>19.1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(C17:C26)</f>
         <v>17.5954539583382</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(D17:D26)</f>
         <v>71.4319939592897</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(E17:E26)</f>
         <v>6.80947729271491</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F17:F26)</f>
+        <v>0.241943587388069</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.P(G17:G26)</f>
         <v>11.9837389824712</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <f aca="false">_xlfn.STDEV.P(G17:G26)</f>
+      <c r="H28" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.P(H17:H26)</f>
         <v>4.15676135952017</v>
       </c>
-      <c r="H28" s="0" t="n">
-        <f aca="false">_xlfn.STDEV.P(H17:H26)</f>
+      <c r="I28" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.P(I17:I26)</f>
         <v>9.5608577021102</v>
       </c>
-      <c r="I28" s="0" t="n">
-        <f aca="false">_xlfn.STDEV.P(I17:I26)</f>
+      <c r="J28" s="2" t="n">
+        <f aca="false">_xlfn.STDEV.P(J17:J26)</f>
         <v>3.88458491991101</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1838,11 +2049,11 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
@@ -1875,19 +2086,19 @@
         <v>5</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,153 +2106,153 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="H3" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="H4" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="H5" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="H6" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="H7" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="H8" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="H9" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="H10" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="H11" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="e">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7" t="e">
         <f aca="false">AVERAGE(C3:C12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D13" s="6" t="e">
+      <c r="D13" s="7" t="e">
         <f aca="false">AVERAGE(D3:D12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E13" s="6" t="e">
+      <c r="E13" s="7" t="e">
         <f aca="false">AVERAGE(E3:E12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F13" s="6" t="e">
+      <c r="F13" s="7" t="e">
         <f aca="false">AVERAGE(F3:F12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G13" s="6" t="e">
+      <c r="G13" s="7" t="e">
         <f aca="false">AVERAGE(G3:G12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H13" s="6" t="e">
+      <c r="H13" s="7" t="e">
         <f aca="false">AVERAGE(H3:H12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="6" t="e">
+      <c r="I13" s="7" t="e">
         <f aca="false">AVERAGE(I3:I12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J13" s="6" t="e">
+      <c r="J13" s="7" t="e">
         <f aca="false">AVERAGE(J3:J12)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="0" t="e">
         <f aca="false">_xlfn.STDEV.P(C3:C12)</f>
@@ -2081,19 +2292,19 @@
         <v>5</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,152 +2312,152 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="H17" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="B18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="B19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="B20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="B21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="B22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="B23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="B24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="B25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="B26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6" t="e">
+      <c r="A27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7" t="e">
         <f aca="false">AVERAGE(C17:C26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D27" s="6" t="e">
+      <c r="D27" s="7" t="e">
         <f aca="false">AVERAGE(D17:D26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E27" s="6" t="e">
+      <c r="E27" s="7" t="e">
         <f aca="false">AVERAGE(E17:E26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F27" s="6" t="e">
+      <c r="F27" s="7" t="e">
         <f aca="false">AVERAGE(F17:F26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G27" s="6" t="e">
+      <c r="G27" s="7" t="e">
         <f aca="false">AVERAGE(G17:G26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H27" s="6" t="e">
+      <c r="H27" s="7" t="e">
         <f aca="false">AVERAGE(H17:H26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I27" s="6" t="e">
+      <c r="I27" s="7" t="e">
         <f aca="false">AVERAGE(I17:I26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J27" s="6" t="e">
+      <c r="J27" s="7" t="e">
         <f aca="false">AVERAGE(J17:J26)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" s="0" t="e">
         <f aca="false">_xlfn.STDEV.P(C17:C26)</f>

</xml_diff>

<commit_message>
Corrected number of completed flights for D2C2 medium 8 simulation.
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Low traffic densit" sheetId="1" state="visible" r:id="rId2"/>
@@ -222,11 +222,11 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
@@ -1133,11 +1133,11 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
@@ -1860,7 +1860,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>1759.18</v>
@@ -1958,7 +1958,7 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7" t="n">
         <f aca="false">AVERAGE(C17:C26)</f>
-        <v>254</v>
+        <v>253.1</v>
       </c>
       <c r="D27" s="7" t="n">
         <f aca="false">AVERAGE(D17:D26)</f>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="C28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(C17:C26)</f>
-        <v>17.5954539583382</v>
+        <v>16.4890873003936</v>
       </c>
       <c r="D28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(D17:D26)</f>
@@ -2053,7 +2053,7 @@
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>

</xml_diff>

<commit_message>
Corrected bug when counting number of completed flights. (Especially affecting D2C2 scenarios.)
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Low traffic densit" sheetId="1" state="visible" r:id="rId2"/>
@@ -222,8 +222,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -718,17 +718,17 @@
         <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>2592.22</v>
+        <v>4443.81</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>267.42</v>
+        <v>458.45</v>
       </c>
       <c r="F17" s="2" t="n">
         <f aca="false">D17/E17</f>
-        <v>9.69344102909281</v>
+        <v>9.69311811538881</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>4</v>
@@ -1047,19 +1047,19 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7" t="n">
         <f aca="false">AVERAGE(C17:C26)</f>
-        <v>38.9</v>
+        <v>37.4</v>
       </c>
       <c r="D27" s="7" t="n">
         <f aca="false">AVERAGE(D17:D26)</f>
-        <v>2613.274</v>
+        <v>2798.433</v>
       </c>
       <c r="E27" s="7" t="n">
         <f aca="false">AVERAGE(E17:E26)</f>
-        <v>271.565</v>
+        <v>290.668</v>
       </c>
       <c r="F27" s="7" t="n">
         <f aca="false">AVERAGE(F17:F26)</f>
-        <v>9.60727900283848</v>
+        <v>9.60724671146808</v>
       </c>
       <c r="G27" s="7" t="n">
         <f aca="false">AVERAGE(G17:G26)</f>
@@ -1084,19 +1084,19 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(C17:C26)</f>
-        <v>7.40877857679658</v>
+        <v>9.15641851380768</v>
       </c>
       <c r="D28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(D17:D26)</f>
-        <v>256.666532808623</v>
+        <v>605.504526342289</v>
       </c>
       <c r="E28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(E17:E26)</f>
-        <v>15.1002491701296</v>
+        <v>57.9135142777573</v>
       </c>
       <c r="F28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F17:F26)</f>
-        <v>0.568436133473986</v>
+        <v>0.568431247068317</v>
       </c>
       <c r="G28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(G17:G26)</f>
@@ -1133,7 +1133,7 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated with correct numbers for D2-C2 scenarios with medium density.
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Low traffic densit" sheetId="1" state="visible" r:id="rId2"/>
@@ -222,8 +222,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -751,17 +751,17 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>2234.42</v>
+        <v>4561.95</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>252.39</v>
+        <v>515.3</v>
       </c>
       <c r="F18" s="2" t="n">
         <f aca="false">D18/E18</f>
-        <v>8.85304489084354</v>
+        <v>8.8529982534446</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>6</v>
@@ -784,17 +784,17 @@
         <v>14</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3028.08</v>
+        <v>4878.58</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>275.35</v>
+        <v>443.61</v>
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">D19/E19</f>
-        <v>10.9972035591066</v>
+        <v>10.9974527174771</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>6</v>
@@ -817,17 +817,17 @@
         <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2514.8</v>
+        <v>4652.38</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>267.29</v>
+        <v>494.49</v>
       </c>
       <c r="F20" s="2" t="n">
         <f aca="false">D20/E20</f>
-        <v>9.40850761345355</v>
+        <v>9.40844102004085</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>6</v>
@@ -850,17 +850,17 @@
         <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>2289.49</v>
+        <v>4578.98</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>249.01</v>
+        <v>498.17</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">D21/E21</f>
-        <v>9.19436970402795</v>
+        <v>9.19160126061385</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>7</v>
@@ -883,17 +883,17 @@
         <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>2836.64</v>
+        <v>4682.81</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>285.38</v>
+        <v>489.22</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">D22/E22</f>
-        <v>9.93986964748756</v>
+        <v>9.57199215077062</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>4</v>
@@ -916,17 +916,17 @@
         <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>2751.56</v>
+        <v>4540.08</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>279.01</v>
+        <v>460.51</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">D23/E23</f>
-        <v>9.86186875022401</v>
+        <v>9.85880871208009</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>2</v>
@@ -949,17 +949,17 @@
         <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>2624.75</v>
+        <v>4374.59</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>279.87</v>
+        <v>466.45</v>
       </c>
       <c r="F24" s="2" t="n">
         <f aca="false">D24/E24</f>
-        <v>9.37846142852039</v>
+        <v>9.37847572087041</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>2</v>
@@ -982,17 +982,17 @@
         <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>2911.88</v>
+        <v>4950.2</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>301.15</v>
+        <v>511.96</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">D25/E25</f>
-        <v>9.66920139465383</v>
+        <v>9.66911477459177</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>4</v>
@@ -1015,17 +1015,17 @@
         <v>14</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>2348.9</v>
+        <v>4885.72</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>258.78</v>
+        <v>538.26</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">D26/E26</f>
-        <v>9.07682201097457</v>
+        <v>9.07687734552075</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>5</v>
@@ -1047,19 +1047,19 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7" t="n">
         <f aca="false">AVERAGE(C17:C26)</f>
-        <v>37.4</v>
+        <v>21.4</v>
       </c>
       <c r="D27" s="7" t="n">
         <f aca="false">AVERAGE(D17:D26)</f>
-        <v>2798.433</v>
+        <v>4654.91</v>
       </c>
       <c r="E27" s="7" t="n">
         <f aca="false">AVERAGE(E17:E26)</f>
-        <v>290.668</v>
+        <v>487.642</v>
       </c>
       <c r="F27" s="7" t="n">
         <f aca="false">AVERAGE(F17:F26)</f>
-        <v>9.60724671146808</v>
+        <v>9.56988800707988</v>
       </c>
       <c r="G27" s="7" t="n">
         <f aca="false">AVERAGE(G17:G26)</f>
@@ -1084,19 +1084,19 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(C17:C26)</f>
-        <v>9.15641851380768</v>
+        <v>2.10713075057055</v>
       </c>
       <c r="D28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(D17:D26)</f>
-        <v>605.504526342289</v>
+        <v>184.93725633306</v>
       </c>
       <c r="E28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(E17:E26)</f>
-        <v>57.9135142777573</v>
+        <v>28.3812828462703</v>
       </c>
       <c r="F28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F17:F26)</f>
-        <v>0.568431247068317</v>
+        <v>0.557606250083387</v>
       </c>
       <c r="G28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(G17:G26)</f>
@@ -1133,8 +1133,8 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1629,17 +1629,17 @@
         <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>266</v>
+        <v>130</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>1924.21</v>
+        <v>3937.23</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>240.13</v>
+        <v>491.33</v>
       </c>
       <c r="F17" s="2" t="n">
         <f aca="false">D17/E17</f>
-        <v>8.01320118269271</v>
+        <v>8.01341257403375</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>77</v>
@@ -1662,17 +1662,17 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>224</v>
+        <v>121</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>1746.93</v>
+        <v>3233.98</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>233.07</v>
+        <v>431.47</v>
       </c>
       <c r="F18" s="2" t="n">
         <f aca="false">D18/E18</f>
-        <v>7.49530184064873</v>
+        <v>7.49526038890305</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>51</v>
@@ -1695,17 +1695,17 @@
         <v>14</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>243</v>
+        <v>135</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>1795.29</v>
+        <v>3231.53</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>231.27</v>
+        <v>416.29</v>
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">D19/E19</f>
-        <v>7.76274484368919</v>
+        <v>7.76268947128204</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>86</v>
@@ -1728,17 +1728,17 @@
         <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>237</v>
+        <v>127</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>1820.76</v>
+        <v>3397.79</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>238.72</v>
+        <v>445.49</v>
       </c>
       <c r="F20" s="2" t="n">
         <f aca="false">D20/E20</f>
-        <v>7.62717828418231</v>
+        <v>7.62708478304788</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>62</v>
@@ -1761,17 +1761,17 @@
         <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>262</v>
+        <v>139</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>1694.28</v>
+        <v>3193.53</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>219.79</v>
+        <v>414.29</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">D21/E21</f>
-        <v>7.70863096592202</v>
+        <v>7.70844094716262</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>66</v>
@@ -1794,17 +1794,17 @@
         <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>232</v>
+        <v>124</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>1836.97</v>
+        <v>3436.9</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>240.77</v>
+        <v>450.48</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">D22/E22</f>
-        <v>7.62956348382274</v>
+        <v>7.62941751021133</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>67</v>
@@ -1827,17 +1827,17 @@
         <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>263</v>
+        <v>131</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>1751.72</v>
+        <v>3516.81</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>241.76</v>
+        <v>485.36</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">D23/E23</f>
-        <v>7.24569821310391</v>
+        <v>7.24577633097083</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>48</v>
@@ -1860,17 +1860,17 @@
         <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>270</v>
+        <v>132</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>1759.18</v>
+        <v>3598.33</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>240.3</v>
+        <v>491.52</v>
       </c>
       <c r="F24" s="2" t="n">
         <f aca="false">D24/E24</f>
-        <v>7.32076570952976</v>
+        <v>7.32082112630208</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>81</v>
@@ -1893,17 +1893,17 @@
         <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>272</v>
+        <v>138</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>1689.13</v>
+        <v>3329.31</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>235.01</v>
+        <v>463.21</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">D25/E25</f>
-        <v>7.1874813837709</v>
+        <v>7.18747436367954</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>55</v>
@@ -1926,17 +1926,17 @@
         <v>14</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>262</v>
+        <v>134</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>1690.66</v>
+        <v>3305.63</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>226.75</v>
+        <v>443.36</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">D26/E26</f>
-        <v>7.45605292171996</v>
+        <v>7.45585979790689</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>64</v>
@@ -1958,19 +1958,19 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7" t="n">
         <f aca="false">AVERAGE(C17:C26)</f>
-        <v>253.1</v>
+        <v>131.1</v>
       </c>
       <c r="D27" s="7" t="n">
         <f aca="false">AVERAGE(D17:D26)</f>
-        <v>1770.913</v>
+        <v>3418.104</v>
       </c>
       <c r="E27" s="7" t="n">
         <f aca="false">AVERAGE(E17:E26)</f>
-        <v>234.757</v>
+        <v>453.28</v>
       </c>
       <c r="F27" s="7" t="n">
         <f aca="false">AVERAGE(F17:F26)</f>
-        <v>7.54466188290822</v>
+        <v>7.54462372935</v>
       </c>
       <c r="G27" s="7" t="n">
         <f aca="false">AVERAGE(G17:G26)</f>
@@ -1995,19 +1995,19 @@
       </c>
       <c r="C28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(C17:C26)</f>
-        <v>16.4890873003936</v>
+        <v>5.52177507691141</v>
       </c>
       <c r="D28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(D17:D26)</f>
-        <v>71.4319939592897</v>
+        <v>212.640964783364</v>
       </c>
       <c r="E28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(E17:E26)</f>
-        <v>6.80947729271491</v>
+        <v>27.5116669796652</v>
       </c>
       <c r="F28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F17:F26)</f>
-        <v>0.241943587388069</v>
+        <v>0.241952548479869</v>
       </c>
       <c r="G28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(G17:G26)</f>

</xml_diff>

<commit_message>
Corrected the counting of completed flights even more. :-) Updated statistics for exercise 3, low and medium density.
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Low traffic densit" sheetId="1" state="visible" r:id="rId2"/>
@@ -222,8 +222,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -659,7 +659,7 @@
       </c>
       <c r="F14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F3:F12)</f>
-        <v>0.594913360081156</v>
+        <v>0.594913360081158</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(G3:G12)</f>
@@ -718,17 +718,17 @@
         <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>4443.81</v>
+        <v>5205.18</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>458.45</v>
+        <v>531.31</v>
       </c>
       <c r="F17" s="2" t="n">
         <f aca="false">D17/E17</f>
-        <v>9.69311811538881</v>
+        <v>9.79687941126649</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>4</v>
@@ -751,17 +751,17 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>4561.95</v>
+        <v>4894.79</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>515.3</v>
+        <v>546.17</v>
       </c>
       <c r="F18" s="2" t="n">
         <f aca="false">D18/E18</f>
-        <v>8.8529982534446</v>
+        <v>8.96202647527327</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>6</v>
@@ -784,17 +784,17 @@
         <v>14</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>4878.58</v>
+        <v>5535.49</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>443.61</v>
+        <v>486.82</v>
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">D19/E19</f>
-        <v>10.9974527174771</v>
+        <v>11.3707119674623</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>6</v>
@@ -817,17 +817,17 @@
         <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>4652.38</v>
+        <v>5415.21</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>494.49</v>
+        <v>550.9</v>
       </c>
       <c r="F20" s="2" t="n">
         <f aca="false">D20/E20</f>
-        <v>9.40844102004085</v>
+        <v>9.82975131602832</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>6</v>
@@ -850,17 +850,17 @@
         <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>4578.98</v>
+        <v>4893.25</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>498.17</v>
+        <v>527.03</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">D21/E21</f>
-        <v>9.19160126061385</v>
+        <v>9.28457583059788</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>7</v>
@@ -883,17 +883,17 @@
         <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>4682.81</v>
+        <v>5725.13</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>489.22</v>
+        <v>559.52</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">D22/E22</f>
-        <v>9.57199215077062</v>
+        <v>10.2322169002002</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>4</v>
@@ -916,17 +916,17 @@
         <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>4540.08</v>
+        <v>4874.37</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>460.51</v>
+        <v>487.55</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">D23/E23</f>
-        <v>9.85880871208009</v>
+        <v>9.997682288996</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>2</v>
@@ -949,17 +949,17 @@
         <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>4374.59</v>
+        <v>4777.01</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>466.45</v>
+        <v>487.64</v>
       </c>
       <c r="F24" s="2" t="n">
         <f aca="false">D24/E24</f>
-        <v>9.37847572087041</v>
+        <v>9.79618160938397</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>2</v>
@@ -982,17 +982,17 @@
         <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>4950.2</v>
+        <v>5344.14</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>511.96</v>
+        <v>524.2</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">D25/E25</f>
-        <v>9.66911477459177</v>
+        <v>10.1948492941625</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>4</v>
@@ -1015,17 +1015,17 @@
         <v>14</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>4885.72</v>
+        <v>5386.7</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>538.26</v>
+        <v>582.38</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">D26/E26</f>
-        <v>9.07687734552075</v>
+        <v>9.24945911604107</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>5</v>
@@ -1047,19 +1047,19 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7" t="n">
         <f aca="false">AVERAGE(C17:C26)</f>
-        <v>21.4</v>
+        <v>18.4</v>
       </c>
       <c r="D27" s="7" t="n">
         <f aca="false">AVERAGE(D17:D26)</f>
-        <v>4654.91</v>
+        <v>5205.127</v>
       </c>
       <c r="E27" s="7" t="n">
         <f aca="false">AVERAGE(E17:E26)</f>
-        <v>487.642</v>
+        <v>528.352</v>
       </c>
       <c r="F27" s="7" t="n">
         <f aca="false">AVERAGE(F17:F26)</f>
-        <v>9.56988800707988</v>
+        <v>9.8714334209412</v>
       </c>
       <c r="G27" s="7" t="n">
         <f aca="false">AVERAGE(G17:G26)</f>
@@ -1084,19 +1084,19 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(C17:C26)</f>
-        <v>2.10713075057055</v>
+        <v>2.49799919935936</v>
       </c>
       <c r="D28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(D17:D26)</f>
-        <v>184.93725633306</v>
+        <v>310.198604995251</v>
       </c>
       <c r="E28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(E17:E26)</f>
-        <v>28.3812828462703</v>
+        <v>31.2910149403946</v>
       </c>
       <c r="F28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F17:F26)</f>
-        <v>0.557606250083387</v>
+        <v>0.637947558675564</v>
       </c>
       <c r="G28" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(G17:G26)</f>
@@ -1133,8 +1133,8 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1258,17 +1258,17 @@
         <v>11</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>3617.58</v>
+        <v>3599.5</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>289.68</v>
+        <v>288.24</v>
       </c>
       <c r="F5" s="2" t="n">
         <f aca="false">D5/E5</f>
-        <v>12.4881938690969</v>
+        <v>12.4878573411046</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>47</v>
@@ -1324,17 +1324,17 @@
         <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>3649.09</v>
+        <v>3630.38</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>291.61</v>
+        <v>290.12</v>
       </c>
       <c r="F7" s="2" t="n">
         <f aca="false">D7/E7</f>
-        <v>12.513596927403</v>
+        <v>12.5133737763684</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>59</v>
@@ -1390,17 +1390,17 @@
         <v>11</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>3659.14</v>
+        <v>3640.57</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>303.29</v>
+        <v>301.75</v>
       </c>
       <c r="F9" s="2" t="n">
         <f aca="false">D9/E9</f>
-        <v>12.0648224471628</v>
+        <v>12.0648550124275</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>57</v>
@@ -1423,17 +1423,17 @@
         <v>11</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>3661.97</v>
+        <v>3643.19</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>304.67</v>
+        <v>303.11</v>
       </c>
       <c r="F10" s="2" t="n">
         <f aca="false">D10/E10</f>
-        <v>12.0194636820166</v>
+        <v>12.0193659067665</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>52</v>
@@ -1456,17 +1456,17 @@
         <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>3686.5</v>
+        <v>3668.37</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>314.03</v>
+        <v>312.48</v>
       </c>
       <c r="F11" s="2" t="n">
         <f aca="false">D11/E11</f>
-        <v>11.739324268382</v>
+        <v>11.7395353302611</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>52</v>
@@ -1489,17 +1489,17 @@
         <v>11</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>3560.19</v>
+        <v>3542.39</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>303.76</v>
+        <v>302.25</v>
       </c>
       <c r="F12" s="2" t="n">
         <f aca="false">D12/E12</f>
-        <v>11.7204042665262</v>
+        <v>11.7200661703888</v>
       </c>
       <c r="G12" s="4" t="n">
         <v>60</v>
@@ -1521,19 +1521,19 @@
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="n">
         <f aca="false">AVERAGE(C3:C12)</f>
-        <v>197.9</v>
+        <v>198.5</v>
       </c>
       <c r="D13" s="7" t="n">
         <f aca="false">AVERAGE(D3:D12)</f>
-        <v>3654.116</v>
+        <v>3643.109</v>
       </c>
       <c r="E13" s="7" t="n">
         <f aca="false">AVERAGE(E3:E12)</f>
-        <v>304.624</v>
+        <v>303.715</v>
       </c>
       <c r="F13" s="7" t="n">
         <f aca="false">AVERAGE(F3:F11)</f>
-        <v>12.0370424950249</v>
+        <v>12.0369965142323</v>
       </c>
       <c r="G13" s="7" t="n">
         <f aca="false">AVERAGE(G3:G12)</f>
@@ -1558,19 +1558,19 @@
       </c>
       <c r="C14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(C3:C12)</f>
-        <v>3.26955654485436</v>
+        <v>3.20156211871642</v>
       </c>
       <c r="D14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(D3:D12)</f>
-        <v>68.2262633008726</v>
+        <v>71.1012370426844</v>
       </c>
       <c r="E14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(E3:E12)</f>
-        <v>10.3382331178978</v>
+        <v>10.6468100856548</v>
       </c>
       <c r="F14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F3:F12)</f>
-        <v>0.349389483439253</v>
+        <v>0.349322217118894</v>
       </c>
       <c r="G14" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(G3:G12)</f>
@@ -1629,17 +1629,17 @@
         <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>3937.23</v>
+        <v>4526.83</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>491.33</v>
+        <v>555.12</v>
       </c>
       <c r="F17" s="2" t="n">
         <f aca="false">D17/E17</f>
-        <v>8.01341257403375</v>
+        <v>8.15468727482346</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>77</v>
@@ -1662,17 +1662,17 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>3233.98</v>
+        <v>3827.7</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>431.47</v>
+        <v>491.3</v>
       </c>
       <c r="F18" s="2" t="n">
         <f aca="false">D18/E18</f>
-        <v>7.49526038890305</v>
+        <v>7.79096275188276</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>51</v>
@@ -1695,17 +1695,17 @@
         <v>14</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3231.53</v>
+        <v>3864.37</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>416.29</v>
+        <v>486.43</v>
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">D19/E19</f>
-        <v>7.76268947128204</v>
+        <v>7.94434964948708</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>86</v>
@@ -1728,17 +1728,17 @@
         <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>3397.79</v>
+        <v>3943.27</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>445.49</v>
+        <v>489.47</v>
       </c>
       <c r="F20" s="2" t="n">
         <f aca="false">D20/E20</f>
-        <v>7.62708478304788</v>
+        <v>8.05620364884467</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>62</v>
@@ -1761,17 +1761,17 @@
         <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>3193.53</v>
+        <v>3945.48</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>414.29</v>
+        <v>475.41</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">D21/E21</f>
-        <v>7.70844094716262</v>
+        <v>8.29911024168612</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>66</v>
@@ -1794,17 +1794,17 @@
         <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>3436.9</v>
+        <v>4044.4</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>450.48</v>
+        <v>512.62</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">D22/E22</f>
-        <v>7.62941751021133</v>
+        <v>7.88966485895985</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>67</v>
@@ -1827,17 +1827,17 @@
         <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>3516.81</v>
+        <v>3933.89</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>485.36</v>
+        <v>527</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">D23/E23</f>
-        <v>7.24577633097083</v>
+        <v>7.46468690702087</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>48</v>
@@ -1860,17 +1860,17 @@
         <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>3598.33</v>
+        <v>4147.57</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>491.52</v>
+        <v>546.67</v>
       </c>
       <c r="F24" s="2" t="n">
         <f aca="false">D24/E24</f>
-        <v>7.32082112630208</v>
+        <v>7.58697203065835</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>81</v>
@@ -1893,17 +1893,17 @@
         <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>3329.31</v>
+        <v>3873.19</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>463.21</v>
+        <v>520.27</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">D25/E25</f>
-        <v>7.18747436367954</v>
+        <v>7.44457685432564</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>55</v>
@@ -1926,17 +1926,17 @@
         <v>14</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>3305.63</v>
+        <v>3740.77</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>443.36</v>
+        <v>477.09</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">D26/E26</f>
-        <v>7.45585979790689</v>
+        <v>7.8408057179987</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>64</v>
@@ -1958,19 +1958,19 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7" t="n">
         <f aca="false">AVERAGE(C17:C26)</f>
-        <v>131.1</v>
+        <v>98</v>
       </c>
       <c r="D27" s="7" t="n">
         <f aca="false">AVERAGE(D17:D26)</f>
-        <v>3418.104</v>
+        <v>3984.747</v>
       </c>
       <c r="E27" s="7" t="n">
         <f aca="false">AVERAGE(E17:E26)</f>
-        <v>453.28</v>
+        <v>508.138</v>
       </c>
       <c r="F27" s="7" t="n">
         <f aca="false">AVERAGE(F17:F26)</f>
-        <v>7.54462372935</v>
+        <v>7.84720199356875</v>
       </c>
       <c r="G27" s="7" t="n">
         <f aca="false">AVERAGE(G17:G26)</f>
@@ -1995,19 +1995,19 @@
       </c>
       <c r="C28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(C17:C26)</f>
-        <v>5.52177507691141</v>
+        <v>6.308724118235</v>
       </c>
       <c r="D28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(D17:D26)</f>
-        <v>212.640964783364</v>
+        <v>209.975375939656</v>
       </c>
       <c r="E28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(E17:E26)</f>
-        <v>27.5116669796652</v>
+        <v>27.1171941026353</v>
       </c>
       <c r="F28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(F17:F26)</f>
-        <v>0.241952548479869</v>
+        <v>0.2707469130444</v>
       </c>
       <c r="G28" s="2" t="n">
         <f aca="false">_xlfn.STDEV.P(G17:G26)</f>

</xml_diff>

<commit_message>
Add analysed results for low density - Reference
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\i04.local\i2\ctx\1\RV\rv350\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3770D17-5660-413F-991E-B13A88DDB703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F72EEEA-291B-47FB-A2BB-A39BD6CFE916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16050" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -548,20 +548,25 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
+      <c r="C3">
+        <v>29</v>
+      </c>
       <c r="D3">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2">
-        <v>4658.53</v>
+        <v>4198.1058266633299</v>
       </c>
       <c r="F3" s="2">
-        <v>370.5</v>
+        <v>397.0416666667</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ref="G3:G12" si="0">E3/F3</f>
-        <v>12.573630229419702</v>
-      </c>
-      <c r="H3" s="2"/>
+        <v>10.573464145231553</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.15324225351739901</v>
+      </c>
       <c r="I3">
         <v>5</v>
       </c>
@@ -582,31 +587,36 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
+      <c r="C4">
+        <v>29</v>
+      </c>
       <c r="D4">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2">
-        <v>4350.87</v>
+        <v>3880.6932524879198</v>
       </c>
       <c r="F4" s="2">
-        <v>331.61</v>
+        <v>329.21458333330003</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>13.120442688700582</v>
-      </c>
-      <c r="H4" s="2"/>
+        <v>11.787731920001455</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.13169847578285401</v>
+      </c>
       <c r="I4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J4" s="2">
-        <v>6.5</v>
+        <v>13.25</v>
       </c>
       <c r="K4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -616,25 +626,30 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
+      <c r="C5">
+        <v>29</v>
+      </c>
       <c r="D5">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2">
-        <v>4563.3999999999996</v>
+        <v>4126.9580694065198</v>
       </c>
       <c r="F5" s="2">
-        <v>343.92</v>
+        <v>355.02608695652202</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>13.268783438008837</v>
-      </c>
-      <c r="H5" s="2"/>
+        <v>11.624379787933512</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.14091564198565101</v>
+      </c>
       <c r="I5">
         <v>3</v>
       </c>
       <c r="J5" s="2">
-        <v>10.67</v>
+        <v>10.666666666999999</v>
       </c>
       <c r="K5" s="3">
         <v>2</v>
@@ -650,20 +665,25 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
+      <c r="C6">
+        <v>28</v>
+      </c>
       <c r="D6">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2">
-        <v>4541</v>
+        <v>4102.6916407434801</v>
       </c>
       <c r="F6" s="2">
-        <v>348.35</v>
+        <v>359.77608695652202</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>13.035739916750394</v>
-      </c>
-      <c r="H6" s="2"/>
+        <v>11.403458399499685</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.14140862703993201</v>
+      </c>
       <c r="I6">
         <v>5</v>
       </c>
@@ -684,25 +704,30 @@
       <c r="B7" t="s">
         <v>13</v>
       </c>
+      <c r="C7">
+        <v>27</v>
+      </c>
       <c r="D7">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2">
-        <v>4617.47</v>
+        <v>4146.7932304936403</v>
       </c>
       <c r="F7" s="2">
-        <v>390.36</v>
+        <v>406.10681818180001</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>11.8287478225228</v>
-      </c>
-      <c r="H7" s="2"/>
+        <v>10.211089902551855</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.14537235922133501</v>
+      </c>
       <c r="I7">
         <v>6</v>
       </c>
       <c r="J7" s="2">
-        <v>13.33</v>
+        <v>13.333299999999999</v>
       </c>
       <c r="K7" s="3">
         <v>5</v>
@@ -718,31 +743,36 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
+      <c r="C8">
+        <v>29</v>
+      </c>
       <c r="D8">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2">
-        <v>5064.1000000000004</v>
+        <v>4561.7258162095504</v>
       </c>
       <c r="F8" s="2">
-        <v>395.9</v>
+        <v>392.35909090000001</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>12.791361454912858</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>11.626405305776872</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.14994554004031199</v>
+      </c>
       <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="2">
+        <v>12.25</v>
+      </c>
+      <c r="K8" s="3">
         <v>3</v>
       </c>
-      <c r="J8" s="2">
-        <v>6</v>
-      </c>
-      <c r="K8" s="3">
-        <v>1</v>
-      </c>
       <c r="L8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -752,31 +782,36 @@
       <c r="B9" t="s">
         <v>13</v>
       </c>
+      <c r="C9">
+        <v>25</v>
+      </c>
       <c r="D9">
-        <v>23</v>
-      </c>
-      <c r="E9">
-        <v>4524.05</v>
+        <v>20</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3890.0932503795002</v>
       </c>
       <c r="F9" s="2">
-        <v>361.99</v>
+        <v>356.41750000000002</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>12.497720931517446</v>
-      </c>
-      <c r="H9" s="2"/>
+        <v>10.914428304949954</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.124329507239932</v>
+      </c>
       <c r="I9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J9" s="2">
-        <v>6.5</v>
+        <v>13.25</v>
       </c>
       <c r="K9" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -786,31 +821,36 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
+      <c r="C10">
+        <v>28</v>
+      </c>
       <c r="D10">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2">
-        <v>4342.3</v>
+        <v>3741.19335725273</v>
       </c>
       <c r="F10" s="2">
-        <v>380.15</v>
+        <v>378.24318181799998</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>11.4225963435486</v>
-      </c>
-      <c r="H10" s="2"/>
+        <v>9.8909736833085535</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.14202403120165299</v>
+      </c>
       <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="K10" s="3">
         <v>3</v>
       </c>
-      <c r="J10" s="2">
-        <v>6.33</v>
-      </c>
-      <c r="K10" s="3">
-        <v>2</v>
-      </c>
       <c r="L10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -820,31 +860,36 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
       <c r="D11">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E11" s="2">
-        <v>4989.6499999999996</v>
+        <v>4424.7157803099999</v>
       </c>
       <c r="F11" s="2">
-        <v>376.24</v>
+        <v>386.71</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>13.261880714437591</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>11.441948179023042</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.139017814957895</v>
+      </c>
       <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2">
+        <v>10.66667</v>
+      </c>
+      <c r="K11" s="3">
         <v>2</v>
       </c>
-      <c r="J11" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="K11" s="3">
-        <v>1</v>
-      </c>
       <c r="L11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -854,31 +899,36 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
+      <c r="C12">
+        <v>29</v>
+      </c>
       <c r="D12">
-        <v>28</v>
-      </c>
-      <c r="E12">
-        <v>4742.6499999999996</v>
+        <v>25</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4272.0677608351998</v>
       </c>
       <c r="F12" s="2">
-        <v>388.91</v>
+        <v>388.47800000000001</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>12.194723714998327</v>
-      </c>
-      <c r="H12" s="2"/>
+        <v>10.996936147826132</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.15280485335514399</v>
+      </c>
       <c r="I12" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12" s="5">
-        <v>6.5</v>
+        <v>11.5</v>
       </c>
       <c r="K12" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -886,83 +936,90 @@
         <v>14</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="7">
+        <f t="shared" ref="C13" si="1">AVERAGE(C3:C12)</f>
+        <v>28</v>
+      </c>
       <c r="D13" s="7">
-        <f t="shared" ref="D13:L13" si="1">AVERAGE(D3:D12)</f>
-        <v>25.2</v>
+        <f t="shared" ref="D13:L13" si="2">AVERAGE(D3:D12)</f>
+        <v>22.5</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="1"/>
-        <v>4639.402</v>
+        <f t="shared" si="2"/>
+        <v>4134.5037984781866</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="1"/>
-        <v>368.79300000000001</v>
+        <f t="shared" si="2"/>
+        <v>374.93730148128441</v>
       </c>
       <c r="G13" s="7">
-        <f t="shared" si="1"/>
-        <v>12.599562725481714</v>
-      </c>
-      <c r="H13" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>11.047081577610262</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="2"/>
+        <v>0.14207591043421069</v>
       </c>
       <c r="I13" s="7">
-        <f t="shared" si="1"/>
-        <v>3.3</v>
+        <f t="shared" si="2"/>
+        <v>4.2</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="1"/>
-        <v>8.4929999999999986</v>
+        <f t="shared" si="2"/>
+        <v>11.701663666699998</v>
       </c>
       <c r="K13" s="7">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <f t="shared" si="2"/>
+        <v>3.2</v>
       </c>
       <c r="L13" s="7">
-        <f t="shared" si="1"/>
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14" si="3">_xlfn.STDEV.P(C3:C12)</f>
+        <v>1.2649110640673518</v>
+      </c>
       <c r="D14" s="2">
-        <f t="shared" ref="D14:L14" si="2">_xlfn.STDEV.P(D3:D12)</f>
-        <v>1.6613247725836149</v>
+        <f t="shared" ref="D14:L14" si="4">_xlfn.STDEV.P(D3:D12)</f>
+        <v>1.5652475842498528</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="2"/>
-        <v>226.89970254718273</v>
+        <f t="shared" si="4"/>
+        <v>238.70067083332552</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="2"/>
-        <v>20.633493184625809</v>
+        <f t="shared" si="4"/>
+        <v>22.707719306868274</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="2"/>
-        <v>0.59491336008115614</v>
-      </c>
-      <c r="H14" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>0.61483889585786478</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="4"/>
+        <v>8.6392545075983929E-3</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="2"/>
-        <v>1.4177446878757824</v>
+        <f t="shared" si="4"/>
+        <v>0.87177978870813466</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="2"/>
-        <v>2.6678869916096537</v>
+        <f t="shared" si="4"/>
+        <v>1.2494274640058269</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="2"/>
-        <v>1.4696938456699069</v>
+        <f t="shared" si="4"/>
+        <v>0.87177978870813466</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="2"/>
-        <v>0.45825756949558399</v>
+        <f t="shared" si="4"/>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1023,7 +1080,7 @@
         <v>579.60312499999998</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" ref="G17:G26" si="3">E17/F17</f>
+        <f t="shared" ref="G17:G26" si="5">E17/F17</f>
         <v>8.1783975354806273</v>
       </c>
       <c r="H17" s="2">
@@ -1062,7 +1119,7 @@
         <v>581.29999999999995</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.7208416881980053</v>
       </c>
       <c r="H18" s="2">
@@ -1101,7 +1158,7 @@
         <v>518.1</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.5731086099743088</v>
       </c>
       <c r="H19" s="2">
@@ -1140,7 +1197,7 @@
         <v>587.00312499999995</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.3787372725517955</v>
       </c>
       <c r="H20" s="2">
@@ -1179,7 +1236,7 @@
         <v>588.52499999999998</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.5923331899116091</v>
       </c>
       <c r="H21" s="2">
@@ -1218,7 +1275,7 @@
         <v>604.04</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.6255680431958162</v>
       </c>
       <c r="H22" s="2">
@@ -1257,7 +1314,7 @@
         <v>520.9</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.2297567108682088</v>
       </c>
       <c r="H23" s="2">
@@ -1296,7 +1353,7 @@
         <v>521.00312499999995</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.0180158631833933</v>
       </c>
       <c r="H24" s="2">
@@ -1335,7 +1392,7 @@
         <v>565.54333333299996</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.4543878665309791</v>
       </c>
       <c r="H25" s="2">
@@ -1374,7 +1431,7 @@
         <v>618.16999999999996</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.0290121352953072</v>
       </c>
       <c r="H26" s="2">
@@ -1399,43 +1456,43 @@
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="7">
-        <f>AVERAGE(C17:C26)</f>
+        <f t="shared" ref="C27:L27" si="6">AVERAGE(C17:C26)</f>
         <v>23.4</v>
       </c>
       <c r="D27" s="7">
-        <f>AVERAGE(D17:D26)</f>
+        <f t="shared" si="6"/>
         <v>16.899999999999999</v>
       </c>
       <c r="E27" s="7">
-        <f>AVERAGE(E17:E26)</f>
+        <f t="shared" si="6"/>
         <v>4699.3897305893543</v>
       </c>
       <c r="F27" s="7">
-        <f>AVERAGE(F17:F26)</f>
+        <f t="shared" si="6"/>
         <v>568.41877083329996</v>
       </c>
       <c r="G27" s="7">
-        <f>AVERAGE(G17:G26)</f>
+        <f t="shared" si="6"/>
         <v>8.280015891519005</v>
       </c>
       <c r="H27" s="7">
-        <f>AVERAGE(H17:H26)</f>
+        <f t="shared" si="6"/>
         <v>0.14657415694464462</v>
       </c>
       <c r="I27" s="7">
-        <f>AVERAGE(I17:I26)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="J27" s="7">
-        <f>AVERAGE(J17:J26)</f>
+        <f t="shared" si="6"/>
         <v>9.1935714652714289</v>
       </c>
       <c r="K27" s="7">
-        <f>AVERAGE(K17:K26)</f>
+        <f t="shared" si="6"/>
         <v>5.3</v>
       </c>
       <c r="L27" s="7">
-        <f>AVERAGE(L17:L26)</f>
+        <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1444,43 +1501,43 @@
         <v>15</v>
       </c>
       <c r="C28" s="2">
-        <f>_xlfn.STDEV.P(C17:C26)</f>
+        <f t="shared" ref="C28:L28" si="7">_xlfn.STDEV.P(C17:C26)</f>
         <v>2.5768197453450252</v>
       </c>
       <c r="D28" s="2">
-        <f>_xlfn.STDEV.P(D17:D26)</f>
+        <f t="shared" si="7"/>
         <v>2.6627053911388696</v>
       </c>
       <c r="E28" s="2">
-        <f>_xlfn.STDEV.P(E17:E26)</f>
+        <f t="shared" si="7"/>
         <v>315.49664468227411</v>
       </c>
       <c r="F28" s="2">
-        <f>_xlfn.STDEV.P(F17:F26)</f>
+        <f t="shared" si="7"/>
         <v>34.396562583056742</v>
       </c>
       <c r="G28" s="2">
-        <f>_xlfn.STDEV.P(G17:G26)</f>
+        <f t="shared" si="7"/>
         <v>0.52552155317863214</v>
       </c>
       <c r="H28" s="2">
-        <f>_xlfn.STDEV.P(H17:H26)</f>
+        <f t="shared" si="7"/>
         <v>2.4276289746912972E-2</v>
       </c>
       <c r="I28" s="2">
-        <f>_xlfn.STDEV.P(I17:I26)</f>
+        <f t="shared" si="7"/>
         <v>1.8973665961010275</v>
       </c>
       <c r="J28" s="2">
-        <f>_xlfn.STDEV.P(J17:J26)</f>
+        <f t="shared" si="7"/>
         <v>4.4047589622140988</v>
       </c>
       <c r="K28" s="2">
-        <f>_xlfn.STDEV.P(K17:K26)</f>
+        <f t="shared" si="7"/>
         <v>2.0024984394500787</v>
       </c>
       <c r="L28" s="2">
-        <f>_xlfn.STDEV.P(L17:L26)</f>
+        <f t="shared" si="7"/>
         <v>0.45825756949558399</v>
       </c>
     </row>
@@ -1506,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add analysed results for medium density - Reference
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\i04.local\i2\ctx\1\RV\rv350\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F72EEEA-291B-47FB-A2BB-A39BD6CFE916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149507B5-4AAE-4187-AC11-C39471F7EA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16050" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16050" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Low traffic densit" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1563,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1629,33 +1629,35 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="D3">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="E3" s="2">
-        <v>3812.39</v>
+        <v>3728.2939018162401</v>
       </c>
       <c r="F3" s="2">
-        <v>313.3</v>
+        <v>313.22747252747303</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ref="G3:G12" si="0">E3/F3</f>
-        <v>12.168496648579636</v>
-      </c>
-      <c r="H3" s="2"/>
+        <v>11.902831739924196</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.943585304942688</v>
+      </c>
       <c r="I3">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="J3" s="2">
-        <v>6.85</v>
+        <v>6.6779661016949197</v>
       </c>
       <c r="K3">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1666,33 +1668,35 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="D4">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="E4" s="2">
-        <v>3562.22</v>
+        <v>3645.57271517038</v>
       </c>
       <c r="F4" s="2">
-        <v>301.95999999999998</v>
+        <v>310.99862637362702</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>11.796992979202544</v>
-      </c>
-      <c r="H4" s="2"/>
+        <v>11.722150537059504</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.98136119459873705</v>
+      </c>
       <c r="I4">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J4" s="2">
-        <v>14.13</v>
+        <v>17.315789473684202</v>
       </c>
       <c r="K4">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="L4">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1703,30 +1707,32 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="D5">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="E5" s="2">
-        <v>3599.5</v>
+        <v>3468.5506895009398</v>
       </c>
       <c r="F5" s="2">
-        <v>288.24</v>
+        <v>292.17750000000001</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>12.487857341104634</v>
-      </c>
-      <c r="H5" s="2"/>
+        <v>11.871381915106193</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.90648305124000605</v>
+      </c>
       <c r="I5">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5" s="2">
-        <v>25.36</v>
+        <v>23.630434782608699</v>
       </c>
       <c r="K5">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -1740,30 +1746,32 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="D6">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E6" s="2">
-        <v>3639.11</v>
+        <v>3556.5964387519298</v>
       </c>
       <c r="F6" s="2">
-        <v>297.92</v>
+        <v>296.99861878452998</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>12.215057733619764</v>
-      </c>
-      <c r="H6" s="2"/>
+        <v>11.975127875366352</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.87445410350742303</v>
+      </c>
       <c r="I6">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J6" s="2">
-        <v>9.58</v>
+        <v>8.2909090899999995</v>
       </c>
       <c r="K6">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L6">
         <v>9</v>
@@ -1777,33 +1785,35 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="D7">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="E7" s="2">
-        <v>3630.38</v>
+        <v>3541.6060530570498</v>
       </c>
       <c r="F7" s="2">
-        <v>290.12</v>
+        <v>291.38852459016402</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>12.5133737763684</v>
-      </c>
-      <c r="H7" s="2"/>
+        <v>12.154239972347211</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.99115935526818999</v>
+      </c>
       <c r="I7">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7" s="2">
-        <v>14.83</v>
+        <v>14.689655172413801</v>
       </c>
       <c r="K7">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L7">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1814,33 +1824,35 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="D8">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="E8" s="2">
-        <v>3692.97</v>
+        <v>3551.55124933562</v>
       </c>
       <c r="F8" s="2">
-        <v>326.02</v>
+        <v>313.60842696629197</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>11.32743389976075</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>11.324795330571128</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.90045219843297897</v>
+      </c>
       <c r="I8">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J8" s="2">
-        <v>7.84</v>
+        <v>9.4166666669999994</v>
       </c>
       <c r="K8">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L8">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1851,33 +1863,35 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="D9">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="E9" s="2">
-        <v>3640.57</v>
+        <v>3519.35645950656</v>
       </c>
       <c r="F9" s="2">
-        <v>301.75</v>
+        <v>298.412568306011</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>12.064855012427508</v>
-      </c>
-      <c r="H9" s="2"/>
+        <v>11.793593277537797</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.88235792606951802</v>
+      </c>
       <c r="I9">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="J9" s="2">
-        <v>8.9499999999999993</v>
+        <v>9.5806451612903203</v>
       </c>
       <c r="K9">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="L9">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1888,33 +1902,35 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="D10">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E10" s="2">
-        <v>3643.19</v>
+        <v>3565.58677805467</v>
       </c>
       <c r="F10" s="2">
-        <v>303.11</v>
+        <v>300.58999999999997</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>12.01936590676652</v>
-      </c>
-      <c r="H10" s="2"/>
+        <v>11.861960737398684</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.91530053560013802</v>
+      </c>
       <c r="I10">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="J10" s="2">
-        <v>9.7100000000000009</v>
+        <v>7.2241379310344804</v>
       </c>
       <c r="K10">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1925,33 +1941,35 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="D11">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="E11" s="2">
-        <v>3668.37</v>
+        <v>3635.7007822218802</v>
       </c>
       <c r="F11" s="2">
-        <v>312.48</v>
+        <v>318.61881720430102</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>11.739535330261136</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>11.410816266669645</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.02991938215926</v>
+      </c>
       <c r="I11">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="J11" s="2">
-        <v>9.7799999999999994</v>
+        <v>10.683333299999999</v>
       </c>
       <c r="K11">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L11">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1962,33 +1980,35 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="D12">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="E12" s="2">
-        <v>3542.39</v>
+        <v>3436.7056426013201</v>
       </c>
       <c r="F12" s="2">
-        <v>302.25</v>
+        <v>301.74725274725301</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>11.720066170388751</v>
-      </c>
-      <c r="H12" s="2"/>
+        <v>11.389351887421968</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.94134338096429204</v>
+      </c>
       <c r="I12" s="4">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J12" s="5">
-        <v>12.26</v>
+        <v>10.0625</v>
       </c>
       <c r="K12">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L12">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1998,43 +2018,43 @@
       <c r="B13" s="6"/>
       <c r="C13" s="7">
         <f t="shared" ref="C13:L13" si="1">AVERAGE(C3:C12)</f>
-        <v>248.5</v>
+        <v>228.3</v>
       </c>
       <c r="D13" s="7">
         <f t="shared" si="1"/>
-        <v>198.5</v>
+        <v>181.7</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="1"/>
-        <v>3643.1090000000004</v>
+        <v>3564.9520710016595</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="1"/>
-        <v>303.71500000000003</v>
+        <v>303.7767807499651</v>
       </c>
       <c r="G13" s="7">
         <f t="shared" si="1"/>
-        <v>12.005303479847964</v>
-      </c>
-      <c r="H13" s="7" t="e">
+        <v>11.740624953940268</v>
+      </c>
+      <c r="H13" s="7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.93664164327832311</v>
       </c>
       <c r="I13" s="7">
         <f t="shared" si="1"/>
-        <v>56.8</v>
+        <v>56.7</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" si="1"/>
-        <v>11.929</v>
+        <v>11.757203767972642</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="1"/>
-        <v>35.1</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="L13" s="7">
         <f t="shared" si="1"/>
-        <v>9.3000000000000007</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -2043,43 +2063,43 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ref="C14:L14" si="2">_xlfn.STDEV.P(C3:C12)</f>
-        <v>2.5787593916455256</v>
+        <v>4.3370496884402874</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="2"/>
-        <v>3.2015621187164243</v>
+        <v>2.0518284528683188</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="2"/>
-        <v>71.101237042684417</v>
+        <v>81.731140123085495</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="2"/>
-        <v>10.64681008565476</v>
+        <v>9.1401474690146856</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="2"/>
-        <v>0.34932221711890077</v>
-      </c>
-      <c r="H14" s="2" t="e">
+        <v>0.26314018332149008</v>
+      </c>
+      <c r="H14" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>4.8199323710887101E-2</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="2"/>
-        <v>5.3999999999999995</v>
+        <v>5.4230987451825001</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="2"/>
-        <v>5.1010988031991698</v>
+        <v>5.0306464882127599</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="2"/>
-        <v>3.0479501308256345</v>
+        <v>3.1953090617340911</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="2"/>
-        <v>2.9681644159311662</v>
+        <v>3.1128764832546763</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add analysed results for high density - reference
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\i04.local\i2\ctx\1\RV\rv350\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149507B5-4AAE-4187-AC11-C39471F7EA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623CA90A-69A4-4E86-B2F7-811A58F1D5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16050" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16050" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Low traffic densit" sheetId="1" r:id="rId1"/>
@@ -1563,7 +1563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -2662,8 +2662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2728,25 +2728,30 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
+      <c r="C3">
+        <v>2400</v>
+      </c>
       <c r="D3">
-        <v>1810</v>
+        <v>1808</v>
       </c>
       <c r="E3" s="2">
-        <v>3749.69</v>
+        <v>3735.70248969963</v>
       </c>
       <c r="F3" s="2">
-        <v>294.64999999999998</v>
+        <v>294.68683628318598</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ref="G3:G12" si="0">E3/F3</f>
-        <v>12.725912099100629</v>
-      </c>
-      <c r="H3" s="2"/>
+        <v>12.676855664193029</v>
+      </c>
+      <c r="H3" s="2">
+        <v>10.485575676776801</v>
+      </c>
       <c r="I3" s="3">
         <v>4933</v>
       </c>
       <c r="J3" s="2">
-        <v>9.5399999999999991</v>
+        <v>9.5449016825461204</v>
       </c>
       <c r="K3" s="3">
         <v>3032</v>
@@ -2762,25 +2767,30 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
+      <c r="C4">
+        <v>2410</v>
+      </c>
       <c r="D4">
-        <v>1791</v>
+        <v>1789</v>
       </c>
       <c r="E4" s="2">
-        <v>3834.49</v>
+        <v>3822.1043566995099</v>
       </c>
       <c r="F4" s="2">
-        <v>301.01</v>
+        <v>301.06950810508698</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>12.738746221055779</v>
-      </c>
-      <c r="H4" s="2"/>
+        <v>12.695089518548725</v>
+      </c>
+      <c r="H4" s="2">
+        <v>10.996842018938599</v>
+      </c>
       <c r="I4" s="3">
         <v>5333</v>
       </c>
       <c r="J4" s="2">
-        <v>9.7100000000000009</v>
+        <v>9.7129195574723397</v>
       </c>
       <c r="K4" s="3">
         <v>3151</v>
@@ -2796,25 +2806,30 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
+      <c r="C5">
+        <v>2421</v>
+      </c>
       <c r="D5">
-        <v>1819</v>
+        <v>1817</v>
       </c>
       <c r="E5" s="2">
-        <v>3753.66</v>
+        <v>3739.3780349748499</v>
       </c>
       <c r="F5" s="2">
-        <v>290.39</v>
+        <v>290.41788662630802</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>12.926271565825269</v>
-      </c>
-      <c r="H5" s="2"/>
+        <v>12.875853062681545</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10.6583477799773</v>
+      </c>
       <c r="I5" s="3">
         <v>4973</v>
       </c>
       <c r="J5" s="2">
-        <v>10</v>
+        <v>10.002614116227599</v>
       </c>
       <c r="K5" s="3">
         <v>2987</v>
@@ -2830,25 +2845,30 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
+      <c r="C6">
+        <v>2398</v>
+      </c>
       <c r="D6">
-        <v>1820</v>
+        <v>1818</v>
       </c>
       <c r="E6" s="2">
-        <v>3753.76</v>
+        <v>3740.6256920923502</v>
       </c>
       <c r="F6" s="2">
-        <v>295.36</v>
+        <v>295.40525302530301</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>12.709100758396533</v>
-      </c>
-      <c r="H6" s="2"/>
+        <v>12.662691857317601</v>
+      </c>
+      <c r="H6" s="2">
+        <v>10.446655875114599</v>
+      </c>
       <c r="I6" s="3">
         <v>4989</v>
       </c>
       <c r="J6" s="2">
-        <v>9.33</v>
+        <v>9.3313289236319896</v>
       </c>
       <c r="K6" s="3">
         <v>2922</v>
@@ -2864,25 +2884,30 @@
       <c r="B7" t="s">
         <v>13</v>
       </c>
+      <c r="C7">
+        <v>2409</v>
+      </c>
       <c r="D7">
-        <v>1807</v>
+        <v>1805</v>
       </c>
       <c r="E7" s="2">
-        <v>3755.72</v>
+        <v>3743.6995201812301</v>
       </c>
       <c r="F7" s="2">
-        <v>291.77</v>
+        <v>291.84487534626101</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>12.872193851321246</v>
-      </c>
-      <c r="H7" s="2"/>
+        <v>12.82770347000096</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10.5704210826934</v>
+      </c>
       <c r="I7" s="3">
         <v>4952</v>
       </c>
       <c r="J7" s="2">
-        <v>9.2100000000000009</v>
+        <v>9.2148626817447497</v>
       </c>
       <c r="K7" s="3">
         <v>2886</v>
@@ -2898,25 +2923,30 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
+      <c r="C8">
+        <v>2409</v>
+      </c>
       <c r="D8">
-        <v>1813</v>
+        <v>1811</v>
       </c>
       <c r="E8" s="2">
-        <v>3759.36</v>
+        <v>3747.3955310451602</v>
       </c>
       <c r="F8" s="2">
-        <v>294.95</v>
+        <v>295.01653782440701</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>12.745753517545348</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>12.7023236008403</v>
+      </c>
+      <c r="H8" s="2">
+        <v>10.6056174365527</v>
+      </c>
       <c r="I8" s="3">
         <v>5140</v>
       </c>
       <c r="J8" s="2">
-        <v>9.0500000000000007</v>
+        <v>9.0470817120622602</v>
       </c>
       <c r="K8" s="3">
         <v>3102</v>
@@ -2932,25 +2962,30 @@
       <c r="B9" t="s">
         <v>13</v>
       </c>
+      <c r="C9">
+        <v>2415</v>
+      </c>
       <c r="D9">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="E9" s="2">
-        <v>3802.5</v>
+        <v>3788.7481489264501</v>
       </c>
       <c r="F9" s="2">
-        <v>295.98</v>
+        <v>296.023679912901</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>12.847151834583418</v>
-      </c>
-      <c r="H9" s="2"/>
+        <v>12.798800927146141</v>
+      </c>
+      <c r="H9" s="2">
+        <v>10.5668559471232</v>
+      </c>
       <c r="I9" s="3">
         <v>4936</v>
       </c>
       <c r="J9" s="2">
-        <v>9.4700000000000006</v>
+        <v>9.4718395461912497</v>
       </c>
       <c r="K9" s="3">
         <v>2918</v>
@@ -2966,25 +3001,30 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
+      <c r="C10">
+        <v>2424</v>
+      </c>
       <c r="D10">
-        <v>1802</v>
+        <v>1800</v>
       </c>
       <c r="E10" s="2">
-        <v>3855.62</v>
+        <v>3839.6599836078799</v>
       </c>
       <c r="F10" s="2">
-        <v>297.17</v>
+        <v>297.17938888899999</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>12.974459063835514</v>
-      </c>
-      <c r="H10" s="2"/>
+        <v>12.92034416640529</v>
+      </c>
+      <c r="H10" s="2">
+        <v>10.972816612706101</v>
+      </c>
       <c r="I10" s="3">
         <v>5269</v>
       </c>
       <c r="J10" s="2">
-        <v>9.52</v>
+        <v>9.5192636173847003</v>
       </c>
       <c r="K10" s="3">
         <v>3079</v>
@@ -3000,25 +3040,30 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
+      <c r="C11">
+        <v>2401</v>
+      </c>
       <c r="D11">
-        <v>1813</v>
+        <v>1811</v>
       </c>
       <c r="E11" s="2">
-        <v>3826.87</v>
+        <v>3811.90502405593</v>
       </c>
       <c r="F11" s="2">
-        <v>295.49</v>
+        <v>295.50935946990597</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>12.950928965447222</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>12.899439228909181</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10.344715637491401</v>
+      </c>
       <c r="I11" s="3">
         <v>4972</v>
       </c>
       <c r="J11" s="2">
-        <v>9.08</v>
+        <v>9.0760257441673406</v>
       </c>
       <c r="K11" s="3">
         <v>2909</v>
@@ -3034,25 +3079,30 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
+      <c r="C12">
+        <v>2412</v>
+      </c>
       <c r="D12">
-        <v>1809</v>
+        <v>1807</v>
       </c>
       <c r="E12" s="2">
-        <v>3761.93</v>
+        <v>3745.0817024089502</v>
       </c>
       <c r="F12" s="2">
-        <v>296.36</v>
+        <v>296.35486995019397</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>12.693784586313942</v>
-      </c>
-      <c r="H12" s="2"/>
+        <v>12.63715255645489</v>
+      </c>
+      <c r="H12" s="2">
+        <v>10.7461598288936</v>
+      </c>
       <c r="I12" s="11">
         <v>5024</v>
       </c>
       <c r="J12" s="5">
-        <v>9.24</v>
+        <v>9.2364649681528697</v>
       </c>
       <c r="K12" s="3">
         <v>2953</v>
@@ -3066,41 +3116,44 @@
         <v>14</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="7">
+        <f t="shared" ref="C13" si="1">AVERAGE(C3:C12)</f>
+        <v>2409.9</v>
+      </c>
       <c r="D13" s="7">
-        <f t="shared" ref="D13:L13" si="1">AVERAGE(D3:D12)</f>
-        <v>1812.3</v>
+        <f t="shared" ref="D13:L13" si="2">AVERAGE(D3:D12)</f>
+        <v>1810.3</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="1"/>
-        <v>3785.3599999999997</v>
+        <f t="shared" si="2"/>
+        <v>3771.4300483691941</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="1"/>
-        <v>295.31299999999999</v>
+        <f t="shared" si="2"/>
+        <v>295.35081954325534</v>
       </c>
       <c r="G13" s="7">
-        <f t="shared" si="1"/>
-        <v>12.818430246342491</v>
-      </c>
-      <c r="H13" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>12.769625405249766</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="2"/>
+        <v>10.639400789626769</v>
       </c>
       <c r="I13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5052.1000000000004</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="1"/>
-        <v>9.4149999999999991</v>
+        <f t="shared" si="2"/>
+        <v>9.4157302549581221</v>
       </c>
       <c r="K13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2993.9</v>
       </c>
       <c r="L13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>600.70000000000005</v>
       </c>
     </row>
@@ -3108,40 +3161,44 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14" si="3">_xlfn.STDEV.P(C3:C12)</f>
+        <v>8.2030482139263334</v>
+      </c>
       <c r="D14" s="2">
-        <f t="shared" ref="D14:L14" si="2">_xlfn.STDEV.P(D3:D12)</f>
+        <f t="shared" ref="D14:L14" si="4">_xlfn.STDEV.P(D3:D12)</f>
         <v>11.925183436744275</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="2"/>
-        <v>38.401012486651908</v>
+        <f t="shared" si="4"/>
+        <v>38.019631480797941</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="2"/>
-        <v>2.7356719467070669</v>
+        <f t="shared" si="4"/>
+        <v>2.7333882058938102</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="2"/>
-        <v>0.10243370702749016</v>
-      </c>
-      <c r="H14" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="4"/>
+        <v>0.10136644274312469</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="4"/>
+        <v>0.20236135989615284</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>137.40629534340849</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="2"/>
-        <v>0.28004463929880885</v>
+        <f t="shared" si="4"/>
+        <v>0.28181822654560257</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>87.499085709508989</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>18.226628870967886</v>
       </c>
     </row>
@@ -3193,7 +3250,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" t="e">
-        <f t="shared" ref="G17:G26" si="3">E17/F17</f>
+        <f t="shared" ref="G17:G26" si="5">E17/F17</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H17" s="2"/>
@@ -3210,7 +3267,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H18" s="2"/>
@@ -3227,7 +3284,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H19" s="2"/>
@@ -3244,7 +3301,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H20" s="2"/>
@@ -3261,7 +3318,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H21" s="2"/>
@@ -3278,7 +3335,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H22" s="2"/>
@@ -3295,7 +3352,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H23" s="2"/>
@@ -3312,7 +3369,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H24" s="2"/>
@@ -3329,7 +3386,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H25" s="2"/>
@@ -3346,7 +3403,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H26" s="2"/>

</xml_diff>

<commit_message>
Add analysed results for medium density - D2C2
</commit_message>
<xml_diff>
--- a/exercise_3/output/exercise_3_statistics.xlsx
+++ b/exercise_3/output/exercise_3_statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\i04.local\i2\ctx\1\RV\rv350\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623CA90A-69A4-4E86-B2F7-811A58F1D5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4622647-C195-4276-84EC-EAFCD457D958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16050" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16050" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Low traffic densit" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="19">
   <si>
     <t>Exercise 3 statistics</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>* Number of simultaneous flights pr. square kilometer, for completed and airborne flights, from the script</t>
-  </si>
-  <si>
-    <t>D2C2 alt</t>
   </si>
   <si>
     <t>https://www.calculator.net/standard-deviation-calculator.html</t>
@@ -1561,9 +1558,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -2148,33 +2145,35 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D17">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E17" s="2">
-        <v>4526.83</v>
+        <v>4169.6757416205901</v>
       </c>
       <c r="F17" s="2">
-        <v>555.12</v>
+        <v>546.12821782178196</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" ref="G17:G27" si="3">E17/F17</f>
-        <v>8.1546872748234609</v>
-      </c>
-      <c r="H17" s="2"/>
+        <f t="shared" ref="G17:G26" si="3">E17/F17</f>
+        <v>7.6349758271990273</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.91120313498790995</v>
+      </c>
       <c r="I17">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="J17" s="2">
-        <v>18.100000000000001</v>
+        <v>7.1016949152542397</v>
       </c>
       <c r="K17">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="L17">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -2185,33 +2184,35 @@
         <v>16</v>
       </c>
       <c r="C18" s="9">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D18">
         <v>85</v>
       </c>
       <c r="E18" s="2">
-        <v>3827.7</v>
+        <v>3666.1062516249399</v>
       </c>
       <c r="F18" s="2">
-        <v>491.3</v>
+        <v>500.32352941176498</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="3"/>
-        <v>7.7909627518827591</v>
-      </c>
-      <c r="H18" s="2"/>
+        <v>7.3274711983568217</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.75650790993554895</v>
+      </c>
       <c r="I18">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="J18" s="2">
-        <v>18.100000000000001</v>
+        <v>7.5833332999999996</v>
       </c>
       <c r="K18">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="L18">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -2222,33 +2223,35 @@
         <v>16</v>
       </c>
       <c r="C19" s="9">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D19">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E19" s="2">
-        <v>3864.37</v>
+        <v>3715.1805563173498</v>
       </c>
       <c r="F19" s="2">
-        <v>486.43</v>
+        <v>496.375</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="3"/>
-        <v>7.9443496494870791</v>
-      </c>
-      <c r="H19" s="2"/>
+        <v>7.4846246412840083</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.87801800158121901</v>
+      </c>
       <c r="I19">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="J19" s="2">
-        <v>18.23</v>
+        <v>8</v>
       </c>
       <c r="K19">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="L19">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -2259,33 +2262,35 @@
         <v>16</v>
       </c>
       <c r="C20" s="9">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D20">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E20" s="2">
-        <v>3943.27</v>
+        <v>3753.1046722368801</v>
       </c>
       <c r="F20" s="2">
-        <v>489.47</v>
+        <v>504.91354166669998</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="3"/>
-        <v>8.0562036488446687</v>
-      </c>
-      <c r="H20" s="2"/>
+        <v>7.4331630319282533</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.79966317231164896</v>
+      </c>
       <c r="I20">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="J20" s="2">
-        <v>16.29</v>
+        <v>6.3333332999999996</v>
       </c>
       <c r="K20">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L20">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -2296,33 +2301,35 @@
         <v>16</v>
       </c>
       <c r="C21" s="9">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D21">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E21" s="2">
-        <v>3945.48</v>
+        <v>3695.9154167349002</v>
       </c>
       <c r="F21" s="2">
-        <v>475.41</v>
+        <v>481.52040816326502</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="3"/>
-        <v>8.2991102416861224</v>
-      </c>
-      <c r="H21" s="2"/>
+        <v>7.6755114717417285</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.84160326539679098</v>
+      </c>
       <c r="I21">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J21" s="2">
-        <v>12.27</v>
+        <v>7.83673469387755</v>
       </c>
       <c r="K21">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="L21">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -2333,33 +2340,35 @@
         <v>16</v>
       </c>
       <c r="C22" s="9">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D22">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E22" s="2">
-        <v>4044.4</v>
+        <v>3861.4096512134502</v>
       </c>
       <c r="F22" s="2">
-        <v>512.62</v>
+        <v>534.59367816092004</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="3"/>
-        <v>7.8896648589598533</v>
-      </c>
-      <c r="H22" s="2"/>
+        <v>7.2230739138129367</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.81070380785793195</v>
+      </c>
       <c r="I22">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J22" s="2">
-        <v>16.16</v>
+        <v>6.1935483870967696</v>
       </c>
       <c r="K22">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="L22">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -2370,33 +2379,35 @@
         <v>16</v>
       </c>
       <c r="C23" s="9">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D23">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E23" s="2">
-        <v>3933.89</v>
+        <v>3765.5085450500001</v>
       </c>
       <c r="F23" s="2">
-        <v>527</v>
+        <v>532.55841584158395</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="3"/>
-        <v>7.464686907020873</v>
-      </c>
-      <c r="H23" s="2"/>
+        <v>7.0706018965064983</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.87573879999048099</v>
+      </c>
       <c r="I23">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J23" s="2">
-        <v>11.19</v>
+        <v>5.8085106382978697</v>
       </c>
       <c r="K23">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="L23">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2407,245 +2418,214 @@
         <v>16</v>
       </c>
       <c r="C24" s="9">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="D24">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E24" s="2">
-        <v>4147.57</v>
+        <v>4002.6993699562099</v>
       </c>
       <c r="F24" s="2">
-        <v>546.66999999999996</v>
+        <v>550.66105263157897</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="3"/>
-        <v>7.5869720306583499</v>
-      </c>
-      <c r="H24" s="2"/>
+        <v>7.2688986279809136</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.88673982697217202</v>
+      </c>
       <c r="I24">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="J24" s="2">
-        <v>10.78</v>
+        <v>5.59649122807018</v>
       </c>
       <c r="K24">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="L24">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25" s="9">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="D25">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E25" s="2">
-        <v>4137.5600000000004</v>
+        <v>3797.5452887718102</v>
       </c>
       <c r="F25" s="2">
-        <v>543.80999999999995</v>
+        <v>532.24190476190495</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" si="3"/>
-        <v>7.6084661922362606</v>
-      </c>
-      <c r="H25" s="2"/>
+        <v>7.1349986816062856</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.98544205208833802</v>
+      </c>
       <c r="I25">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J25" s="2">
-        <v>5.6</v>
+        <v>5.5344827586206904</v>
       </c>
       <c r="K25">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L25">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="9">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="D26">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E26" s="2">
-        <v>3873.19</v>
+        <v>3626.4529817215798</v>
       </c>
       <c r="F26" s="2">
-        <v>520.27</v>
+        <v>487.112871287129</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="3"/>
-        <v>7.4445768543256392</v>
-      </c>
-      <c r="H26" s="2"/>
+        <v>7.4447898946689195</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.85595036482068398</v>
+      </c>
       <c r="I26">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J26" s="2">
-        <v>7.13</v>
+        <v>5</v>
       </c>
       <c r="K26">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="L26">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>10</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="9">
-        <v>176</v>
-      </c>
-      <c r="D27">
-        <v>104</v>
-      </c>
-      <c r="E27" s="2">
-        <v>3740.77</v>
-      </c>
-      <c r="F27" s="2">
-        <v>477.09</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="3"/>
-        <v>7.840805717998701</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27">
-        <v>64</v>
-      </c>
-      <c r="J27" s="2">
-        <v>7.3</v>
-      </c>
-      <c r="K27">
-        <v>40</v>
-      </c>
-      <c r="L27">
-        <v>24</v>
+      <c r="A27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7">
+        <f>AVERAGE(C17:C26)</f>
+        <v>165.1</v>
+      </c>
+      <c r="D27" s="7">
+        <f>AVERAGE(D17:D26)</f>
+        <v>96.7</v>
+      </c>
+      <c r="E27" s="7">
+        <f>AVERAGE(E17:E26)</f>
+        <v>3805.3598475247718</v>
+      </c>
+      <c r="F27" s="7">
+        <f>AVERAGE(F17:F26)</f>
+        <v>516.64286197466288</v>
+      </c>
+      <c r="G27" s="7">
+        <f>AVERAGE(G17:G26)</f>
+        <v>7.3698109185085388</v>
+      </c>
+      <c r="H27" s="7">
+        <f>AVERAGE(H17:H26)</f>
+        <v>0.86015703359427254</v>
+      </c>
+      <c r="I27" s="7">
+        <f>AVERAGE(I17:I26)</f>
+        <v>52.7</v>
+      </c>
+      <c r="J27" s="7">
+        <f>AVERAGE(J17:J26)</f>
+        <v>6.4988129221217292</v>
+      </c>
+      <c r="K27" s="7">
+        <f>AVERAGE(K17:K26)</f>
+        <v>60.3</v>
+      </c>
+      <c r="L27" s="7">
+        <f>AVERAGE(L17:L26)</f>
+        <v>20.7</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7">
-        <f>AVERAGE(C18:C27)</f>
-        <v>174.5</v>
-      </c>
-      <c r="D28" s="7">
-        <f>AVERAGE(D17:D27)</f>
-        <v>97.909090909090907</v>
-      </c>
-      <c r="E28" s="7">
-        <f>AVERAGE(E17:E27)</f>
-        <v>3998.639090909091</v>
-      </c>
-      <c r="F28" s="7">
-        <f>AVERAGE(F17:F27)</f>
-        <v>511.38090909090914</v>
-      </c>
-      <c r="G28" s="7">
-        <f>AVERAGE(G17:G27)</f>
-        <v>7.8254987389021604</v>
-      </c>
-      <c r="H28" s="7" t="e">
-        <f>AVERAGE(H17:H26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" s="7">
-        <f>AVERAGE(I17:I27)</f>
-        <v>64.909090909090907</v>
-      </c>
-      <c r="J28" s="7">
-        <f>AVERAGE(J17:J27)</f>
-        <v>12.831818181818182</v>
-      </c>
-      <c r="K28" s="7">
-        <f>AVERAGE(K17:K27)</f>
-        <v>49.272727272727273</v>
-      </c>
-      <c r="L28" s="7">
-        <f>AVERAGE(L17:L27)</f>
-        <v>19.545454545454547</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A28" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="2">
-        <f>_xlfn.STDEV.P(C18:C27)</f>
-        <v>9.1787798753429097</v>
-      </c>
-      <c r="D29" s="2">
-        <f>_xlfn.STDEV.P(D17:D27)</f>
-        <v>6.0219982406106149</v>
-      </c>
-      <c r="E29" s="2">
-        <f>_xlfn.STDEV.P(E17:E27)</f>
-        <v>204.96685006714205</v>
-      </c>
-      <c r="F29" s="2">
-        <f>_xlfn.STDEV.P(F17:F27)</f>
-        <v>27.814699663224321</v>
-      </c>
-      <c r="G29" s="2">
-        <f>_xlfn.STDEV.P(G17:G27)</f>
-        <v>0.2671146073699171</v>
-      </c>
-      <c r="H29" s="2" t="e">
+      <c r="C28" s="2">
+        <f>_xlfn.STDEV.P(C17:C26)</f>
+        <v>11.802118453904791</v>
+      </c>
+      <c r="D28" s="2">
+        <f>_xlfn.STDEV.P(D17:D26)</f>
+        <v>6.0174745533321525</v>
+      </c>
+      <c r="E28" s="2">
+        <f>_xlfn.STDEV.P(E17:E26)</f>
+        <v>158.33507314420186</v>
+      </c>
+      <c r="F28" s="2">
+        <f>_xlfn.STDEV.P(F17:F26)</f>
+        <v>24.012041163700033</v>
+      </c>
+      <c r="G28" s="2">
+        <f>_xlfn.STDEV.P(G17:G26)</f>
+        <v>0.19098515685828341</v>
+      </c>
+      <c r="H28" s="2">
         <f>_xlfn.STDEV.P(H17:H26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I29" s="2">
-        <f>_xlfn.STDEV.P(I17:I27)</f>
-        <v>11.696577164084026</v>
-      </c>
-      <c r="J29" s="2">
-        <f>_xlfn.STDEV.P(J17:J27)</f>
-        <v>4.5757837245891375</v>
-      </c>
-      <c r="K29" s="2">
-        <f>_xlfn.STDEV.P(K17:K27)</f>
-        <v>12.218398266481049</v>
-      </c>
-      <c r="L29" s="2">
-        <f>_xlfn.STDEV.P(L17:L27)</f>
-        <v>3.962635403218794</v>
+        <v>6.0647092965867185E-2</v>
+      </c>
+      <c r="I28" s="2">
+        <f>_xlfn.STDEV.P(I17:I26)</f>
+        <v>8.9</v>
+      </c>
+      <c r="J28" s="2">
+        <f>_xlfn.STDEV.P(J17:J26)</f>
+        <v>1.0085084492383163</v>
+      </c>
+      <c r="K28" s="2">
+        <f>_xlfn.STDEV.P(K17:K26)</f>
+        <v>10.169070754006976</v>
+      </c>
+      <c r="L28" s="2">
+        <f>_xlfn.STDEV.P(L17:L26)</f>
+        <v>3.6891733491393435</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>19</v>
+      <c r="A31" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2662,7 +2642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>